<commit_message>
add filter to package list
</commit_message>
<xml_diff>
--- a/Data/Tests/CliftonTestQuestionsSource.xlsx
+++ b/Data/Tests/CliftonTestQuestionsSource.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RiderProjects\ISarv-Project\iSarv\Data\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B54543-1C80-4804-AD79-9850E4A8F2C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3561CDE2-FC35-400C-BEED-8E81B21E977E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1269,7 +1270,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1558,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5308,7 +5359,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G178">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5337,10 +5388,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA82D3D-61EE-40D7-A850-56F5C1EF6F9F}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A2" sqref="A2:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6577,10 +6628,3264 @@
         <v>308</v>
       </c>
     </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <f>AVERAGE(H2:H35)</f>
+        <v>10.264705882352942</v>
+      </c>
+      <c r="J37">
+        <f>AVERAGE(J2:J35)</f>
+        <v>9.0588235294117645</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <f>STDEV(H2:H35)</f>
+        <v>4.3086159173213217</v>
+      </c>
+      <c r="J38">
+        <f>STDEV(J2:J35)</f>
+        <v>1.7912443020795972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <f>MAX(H2:H35)</f>
+        <v>21</v>
+      </c>
+      <c r="J39">
+        <f>MAX(J2:J35)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <f>MIN(H2:H35)</f>
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <f>MIN(J2:J35)</f>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A178">
     <sortCondition ref="A2:A178"/>
   </sortState>
+  <conditionalFormatting sqref="H2:H35">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>$J$40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>$J$39</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A24B87-9B03-496B-929D-EA612901E726}">
+  <dimension ref="G2:J178"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G2" t="b">
+        <f>TRIM(B2)=TRIM(IF(RIGHT(Sheet1!B2, 1) = ".", LEFT(Sheet1!B2, LEN(Sheet1!B2)-1),Sheet1!B2))</f>
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <f>TRIM(C2)=TRIM(IF(RIGHT(Sheet1!C2, 1) = ".", LEFT(Sheet1!C2, LEN(Sheet1!C2)-1),Sheet1!C2))</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <f>TRIM(D2)=TRIM(IF(RIGHT(Sheet1!D2, 1) = ".", LEFT(Sheet1!D2, LEN(Sheet1!D2)-1),Sheet1!D2))</f>
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <f>TRIM(E2)=TRIM(IF(RIGHT(Sheet1!E2, 1) = ".", LEFT(Sheet1!E2, LEN(Sheet1!E2)-1),Sheet1!E2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G3" t="b">
+        <f>TRIM(B3)=TRIM(IF(RIGHT(Sheet1!B3, 1) = ".", LEFT(Sheet1!B3, LEN(Sheet1!B3)-1),Sheet1!B3))</f>
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <f>TRIM(C3)=TRIM(IF(RIGHT(Sheet1!C3, 1) = ".", LEFT(Sheet1!C3, LEN(Sheet1!C3)-1),Sheet1!C3))</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <f>TRIM(D3)=TRIM(IF(RIGHT(Sheet1!D3, 1) = ".", LEFT(Sheet1!D3, LEN(Sheet1!D3)-1),Sheet1!D3))</f>
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <f>TRIM(E3)=TRIM(IF(RIGHT(Sheet1!E3, 1) = ".", LEFT(Sheet1!E3, LEN(Sheet1!E3)-1),Sheet1!E3))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G4" t="b">
+        <f>TRIM(B4)=TRIM(IF(RIGHT(Sheet1!B4, 1) = ".", LEFT(Sheet1!B4, LEN(Sheet1!B4)-1),Sheet1!B4))</f>
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <f>TRIM(C4)=TRIM(IF(RIGHT(Sheet1!C4, 1) = ".", LEFT(Sheet1!C4, LEN(Sheet1!C4)-1),Sheet1!C4))</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <f>TRIM(D4)=TRIM(IF(RIGHT(Sheet1!D4, 1) = ".", LEFT(Sheet1!D4, LEN(Sheet1!D4)-1),Sheet1!D4))</f>
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <f>TRIM(E4)=TRIM(IF(RIGHT(Sheet1!E4, 1) = ".", LEFT(Sheet1!E4, LEN(Sheet1!E4)-1),Sheet1!E4))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G5" t="b">
+        <f>TRIM(B5)=TRIM(IF(RIGHT(Sheet1!B5, 1) = ".", LEFT(Sheet1!B5, LEN(Sheet1!B5)-1),Sheet1!B5))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <f>TRIM(C5)=TRIM(IF(RIGHT(Sheet1!C5, 1) = ".", LEFT(Sheet1!C5, LEN(Sheet1!C5)-1),Sheet1!C5))</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <f>TRIM(D5)=TRIM(IF(RIGHT(Sheet1!D5, 1) = ".", LEFT(Sheet1!D5, LEN(Sheet1!D5)-1),Sheet1!D5))</f>
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <f>TRIM(E5)=TRIM(IF(RIGHT(Sheet1!E5, 1) = ".", LEFT(Sheet1!E5, LEN(Sheet1!E5)-1),Sheet1!E5))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G6" t="b">
+        <f>TRIM(B6)=TRIM(IF(RIGHT(Sheet1!B6, 1) = ".", LEFT(Sheet1!B6, LEN(Sheet1!B6)-1),Sheet1!B6))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <f>TRIM(C6)=TRIM(IF(RIGHT(Sheet1!C6, 1) = ".", LEFT(Sheet1!C6, LEN(Sheet1!C6)-1),Sheet1!C6))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <f>TRIM(D6)=TRIM(IF(RIGHT(Sheet1!D6, 1) = ".", LEFT(Sheet1!D6, LEN(Sheet1!D6)-1),Sheet1!D6))</f>
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <f>TRIM(E6)=TRIM(IF(RIGHT(Sheet1!E6, 1) = ".", LEFT(Sheet1!E6, LEN(Sheet1!E6)-1),Sheet1!E6))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G7" t="b">
+        <f>TRIM(B7)=TRIM(IF(RIGHT(Sheet1!B7, 1) = ".", LEFT(Sheet1!B7, LEN(Sheet1!B7)-1),Sheet1!B7))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <f>TRIM(C7)=TRIM(IF(RIGHT(Sheet1!C7, 1) = ".", LEFT(Sheet1!C7, LEN(Sheet1!C7)-1),Sheet1!C7))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <f>TRIM(D7)=TRIM(IF(RIGHT(Sheet1!D7, 1) = ".", LEFT(Sheet1!D7, LEN(Sheet1!D7)-1),Sheet1!D7))</f>
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <f>TRIM(E7)=TRIM(IF(RIGHT(Sheet1!E7, 1) = ".", LEFT(Sheet1!E7, LEN(Sheet1!E7)-1),Sheet1!E7))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G8" t="b">
+        <f>TRIM(B8)=TRIM(IF(RIGHT(Sheet1!B8, 1) = ".", LEFT(Sheet1!B8, LEN(Sheet1!B8)-1),Sheet1!B8))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <f>TRIM(C8)=TRIM(IF(RIGHT(Sheet1!C8, 1) = ".", LEFT(Sheet1!C8, LEN(Sheet1!C8)-1),Sheet1!C8))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <f>TRIM(D8)=TRIM(IF(RIGHT(Sheet1!D8, 1) = ".", LEFT(Sheet1!D8, LEN(Sheet1!D8)-1),Sheet1!D8))</f>
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <f>TRIM(E8)=TRIM(IF(RIGHT(Sheet1!E8, 1) = ".", LEFT(Sheet1!E8, LEN(Sheet1!E8)-1),Sheet1!E8))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G9" t="b">
+        <f>TRIM(B9)=TRIM(IF(RIGHT(Sheet1!B9, 1) = ".", LEFT(Sheet1!B9, LEN(Sheet1!B9)-1),Sheet1!B9))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <f>TRIM(C9)=TRIM(IF(RIGHT(Sheet1!C9, 1) = ".", LEFT(Sheet1!C9, LEN(Sheet1!C9)-1),Sheet1!C9))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <f>TRIM(D9)=TRIM(IF(RIGHT(Sheet1!D9, 1) = ".", LEFT(Sheet1!D9, LEN(Sheet1!D9)-1),Sheet1!D9))</f>
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <f>TRIM(E9)=TRIM(IF(RIGHT(Sheet1!E9, 1) = ".", LEFT(Sheet1!E9, LEN(Sheet1!E9)-1),Sheet1!E9))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G10" t="b">
+        <f>TRIM(B10)=TRIM(IF(RIGHT(Sheet1!B10, 1) = ".", LEFT(Sheet1!B10, LEN(Sheet1!B10)-1),Sheet1!B10))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <f>TRIM(C10)=TRIM(IF(RIGHT(Sheet1!C10, 1) = ".", LEFT(Sheet1!C10, LEN(Sheet1!C10)-1),Sheet1!C10))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <f>TRIM(D10)=TRIM(IF(RIGHT(Sheet1!D10, 1) = ".", LEFT(Sheet1!D10, LEN(Sheet1!D10)-1),Sheet1!D10))</f>
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <f>TRIM(E10)=TRIM(IF(RIGHT(Sheet1!E10, 1) = ".", LEFT(Sheet1!E10, LEN(Sheet1!E10)-1),Sheet1!E10))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G11" t="b">
+        <f>TRIM(B11)=TRIM(IF(RIGHT(Sheet1!B11, 1) = ".", LEFT(Sheet1!B11, LEN(Sheet1!B11)-1),Sheet1!B11))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <f>TRIM(C11)=TRIM(IF(RIGHT(Sheet1!C11, 1) = ".", LEFT(Sheet1!C11, LEN(Sheet1!C11)-1),Sheet1!C11))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <f>TRIM(D11)=TRIM(IF(RIGHT(Sheet1!D11, 1) = ".", LEFT(Sheet1!D11, LEN(Sheet1!D11)-1),Sheet1!D11))</f>
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <f>TRIM(E11)=TRIM(IF(RIGHT(Sheet1!E11, 1) = ".", LEFT(Sheet1!E11, LEN(Sheet1!E11)-1),Sheet1!E11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G12" t="b">
+        <f>TRIM(B12)=TRIM(IF(RIGHT(Sheet1!B12, 1) = ".", LEFT(Sheet1!B12, LEN(Sheet1!B12)-1),Sheet1!B12))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <f>TRIM(C12)=TRIM(IF(RIGHT(Sheet1!C12, 1) = ".", LEFT(Sheet1!C12, LEN(Sheet1!C12)-1),Sheet1!C12))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <f>TRIM(D12)=TRIM(IF(RIGHT(Sheet1!D12, 1) = ".", LEFT(Sheet1!D12, LEN(Sheet1!D12)-1),Sheet1!D12))</f>
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <f>TRIM(E12)=TRIM(IF(RIGHT(Sheet1!E12, 1) = ".", LEFT(Sheet1!E12, LEN(Sheet1!E12)-1),Sheet1!E12))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G13" t="b">
+        <f>TRIM(B13)=TRIM(IF(RIGHT(Sheet1!B13, 1) = ".", LEFT(Sheet1!B13, LEN(Sheet1!B13)-1),Sheet1!B13))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <f>TRIM(C13)=TRIM(IF(RIGHT(Sheet1!C13, 1) = ".", LEFT(Sheet1!C13, LEN(Sheet1!C13)-1),Sheet1!C13))</f>
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <f>TRIM(D13)=TRIM(IF(RIGHT(Sheet1!D13, 1) = ".", LEFT(Sheet1!D13, LEN(Sheet1!D13)-1),Sheet1!D13))</f>
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <f>TRIM(E13)=TRIM(IF(RIGHT(Sheet1!E13, 1) = ".", LEFT(Sheet1!E13, LEN(Sheet1!E13)-1),Sheet1!E13))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G14" t="b">
+        <f>TRIM(B14)=TRIM(IF(RIGHT(Sheet1!B14, 1) = ".", LEFT(Sheet1!B14, LEN(Sheet1!B14)-1),Sheet1!B14))</f>
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <f>TRIM(C14)=TRIM(IF(RIGHT(Sheet1!C14, 1) = ".", LEFT(Sheet1!C14, LEN(Sheet1!C14)-1),Sheet1!C14))</f>
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <f>TRIM(D14)=TRIM(IF(RIGHT(Sheet1!D14, 1) = ".", LEFT(Sheet1!D14, LEN(Sheet1!D14)-1),Sheet1!D14))</f>
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <f>TRIM(E14)=TRIM(IF(RIGHT(Sheet1!E14, 1) = ".", LEFT(Sheet1!E14, LEN(Sheet1!E14)-1),Sheet1!E14))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G15" t="b">
+        <f>TRIM(B15)=TRIM(IF(RIGHT(Sheet1!B15, 1) = ".", LEFT(Sheet1!B15, LEN(Sheet1!B15)-1),Sheet1!B15))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <f>TRIM(C15)=TRIM(IF(RIGHT(Sheet1!C15, 1) = ".", LEFT(Sheet1!C15, LEN(Sheet1!C15)-1),Sheet1!C15))</f>
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <f>TRIM(D15)=TRIM(IF(RIGHT(Sheet1!D15, 1) = ".", LEFT(Sheet1!D15, LEN(Sheet1!D15)-1),Sheet1!D15))</f>
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <f>TRIM(E15)=TRIM(IF(RIGHT(Sheet1!E15, 1) = ".", LEFT(Sheet1!E15, LEN(Sheet1!E15)-1),Sheet1!E15))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G16" t="b">
+        <f>TRIM(B16)=TRIM(IF(RIGHT(Sheet1!B16, 1) = ".", LEFT(Sheet1!B16, LEN(Sheet1!B16)-1),Sheet1!B16))</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <f>TRIM(C16)=TRIM(IF(RIGHT(Sheet1!C16, 1) = ".", LEFT(Sheet1!C16, LEN(Sheet1!C16)-1),Sheet1!C16))</f>
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <f>TRIM(D16)=TRIM(IF(RIGHT(Sheet1!D16, 1) = ".", LEFT(Sheet1!D16, LEN(Sheet1!D16)-1),Sheet1!D16))</f>
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <f>TRIM(E16)=TRIM(IF(RIGHT(Sheet1!E16, 1) = ".", LEFT(Sheet1!E16, LEN(Sheet1!E16)-1),Sheet1!E16))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" t="b">
+        <f>TRIM(B17)=TRIM(IF(RIGHT(Sheet1!B17, 1) = ".", LEFT(Sheet1!B17, LEN(Sheet1!B17)-1),Sheet1!B17))</f>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f>TRIM(C17)=TRIM(IF(RIGHT(Sheet1!C17, 1) = ".", LEFT(Sheet1!C17, LEN(Sheet1!C17)-1),Sheet1!C17))</f>
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <f>TRIM(D17)=TRIM(IF(RIGHT(Sheet1!D17, 1) = ".", LEFT(Sheet1!D17, LEN(Sheet1!D17)-1),Sheet1!D17))</f>
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <f>TRIM(E17)=TRIM(IF(RIGHT(Sheet1!E17, 1) = ".", LEFT(Sheet1!E17, LEN(Sheet1!E17)-1),Sheet1!E17))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G18" t="b">
+        <f>TRIM(B18)=TRIM(IF(RIGHT(Sheet1!B18, 1) = ".", LEFT(Sheet1!B18, LEN(Sheet1!B18)-1),Sheet1!B18))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f>TRIM(C18)=TRIM(IF(RIGHT(Sheet1!C18, 1) = ".", LEFT(Sheet1!C18, LEN(Sheet1!C18)-1),Sheet1!C18))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <f>TRIM(D18)=TRIM(IF(RIGHT(Sheet1!D18, 1) = ".", LEFT(Sheet1!D18, LEN(Sheet1!D18)-1),Sheet1!D18))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <f>TRIM(E18)=TRIM(IF(RIGHT(Sheet1!E18, 1) = ".", LEFT(Sheet1!E18, LEN(Sheet1!E18)-1),Sheet1!E18))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G19" t="b">
+        <f>TRIM(B19)=TRIM(IF(RIGHT(Sheet1!B19, 1) = ".", LEFT(Sheet1!B19, LEN(Sheet1!B19)-1),Sheet1!B19))</f>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f>TRIM(C19)=TRIM(IF(RIGHT(Sheet1!C19, 1) = ".", LEFT(Sheet1!C19, LEN(Sheet1!C19)-1),Sheet1!C19))</f>
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <f>TRIM(D19)=TRIM(IF(RIGHT(Sheet1!D19, 1) = ".", LEFT(Sheet1!D19, LEN(Sheet1!D19)-1),Sheet1!D19))</f>
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <f>TRIM(E19)=TRIM(IF(RIGHT(Sheet1!E19, 1) = ".", LEFT(Sheet1!E19, LEN(Sheet1!E19)-1),Sheet1!E19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G20" t="b">
+        <f>TRIM(B20)=TRIM(IF(RIGHT(Sheet1!B20, 1) = ".", LEFT(Sheet1!B20, LEN(Sheet1!B20)-1),Sheet1!B20))</f>
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <f>TRIM(C20)=TRIM(IF(RIGHT(Sheet1!C20, 1) = ".", LEFT(Sheet1!C20, LEN(Sheet1!C20)-1),Sheet1!C20))</f>
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <f>TRIM(D20)=TRIM(IF(RIGHT(Sheet1!D20, 1) = ".", LEFT(Sheet1!D20, LEN(Sheet1!D20)-1),Sheet1!D20))</f>
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <f>TRIM(E20)=TRIM(IF(RIGHT(Sheet1!E20, 1) = ".", LEFT(Sheet1!E20, LEN(Sheet1!E20)-1),Sheet1!E20))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G21" t="b">
+        <f>TRIM(B21)=TRIM(IF(RIGHT(Sheet1!B21, 1) = ".", LEFT(Sheet1!B21, LEN(Sheet1!B21)-1),Sheet1!B21))</f>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f>TRIM(C21)=TRIM(IF(RIGHT(Sheet1!C21, 1) = ".", LEFT(Sheet1!C21, LEN(Sheet1!C21)-1),Sheet1!C21))</f>
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <f>TRIM(D21)=TRIM(IF(RIGHT(Sheet1!D21, 1) = ".", LEFT(Sheet1!D21, LEN(Sheet1!D21)-1),Sheet1!D21))</f>
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <f>TRIM(E21)=TRIM(IF(RIGHT(Sheet1!E21, 1) = ".", LEFT(Sheet1!E21, LEN(Sheet1!E21)-1),Sheet1!E21))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G22" t="b">
+        <f>TRIM(B22)=TRIM(IF(RIGHT(Sheet1!B22, 1) = ".", LEFT(Sheet1!B22, LEN(Sheet1!B22)-1),Sheet1!B22))</f>
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <f>TRIM(C22)=TRIM(IF(RIGHT(Sheet1!C22, 1) = ".", LEFT(Sheet1!C22, LEN(Sheet1!C22)-1),Sheet1!C22))</f>
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <f>TRIM(D22)=TRIM(IF(RIGHT(Sheet1!D22, 1) = ".", LEFT(Sheet1!D22, LEN(Sheet1!D22)-1),Sheet1!D22))</f>
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <f>TRIM(E22)=TRIM(IF(RIGHT(Sheet1!E22, 1) = ".", LEFT(Sheet1!E22, LEN(Sheet1!E22)-1),Sheet1!E22))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G23" t="b">
+        <f>TRIM(B23)=TRIM(IF(RIGHT(Sheet1!B23, 1) = ".", LEFT(Sheet1!B23, LEN(Sheet1!B23)-1),Sheet1!B23))</f>
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <f>TRIM(C23)=TRIM(IF(RIGHT(Sheet1!C23, 1) = ".", LEFT(Sheet1!C23, LEN(Sheet1!C23)-1),Sheet1!C23))</f>
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <f>TRIM(D23)=TRIM(IF(RIGHT(Sheet1!D23, 1) = ".", LEFT(Sheet1!D23, LEN(Sheet1!D23)-1),Sheet1!D23))</f>
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <f>TRIM(E23)=TRIM(IF(RIGHT(Sheet1!E23, 1) = ".", LEFT(Sheet1!E23, LEN(Sheet1!E23)-1),Sheet1!E23))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G24" t="b">
+        <f>TRIM(B24)=TRIM(IF(RIGHT(Sheet1!B24, 1) = ".", LEFT(Sheet1!B24, LEN(Sheet1!B24)-1),Sheet1!B24))</f>
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <f>TRIM(C24)=TRIM(IF(RIGHT(Sheet1!C24, 1) = ".", LEFT(Sheet1!C24, LEN(Sheet1!C24)-1),Sheet1!C24))</f>
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <f>TRIM(D24)=TRIM(IF(RIGHT(Sheet1!D24, 1) = ".", LEFT(Sheet1!D24, LEN(Sheet1!D24)-1),Sheet1!D24))</f>
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <f>TRIM(E24)=TRIM(IF(RIGHT(Sheet1!E24, 1) = ".", LEFT(Sheet1!E24, LEN(Sheet1!E24)-1),Sheet1!E24))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G25" t="b">
+        <f>TRIM(B25)=TRIM(IF(RIGHT(Sheet1!B25, 1) = ".", LEFT(Sheet1!B25, LEN(Sheet1!B25)-1),Sheet1!B25))</f>
+        <v>0</v>
+      </c>
+      <c r="H25" t="b">
+        <f>TRIM(C25)=TRIM(IF(RIGHT(Sheet1!C25, 1) = ".", LEFT(Sheet1!C25, LEN(Sheet1!C25)-1),Sheet1!C25))</f>
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <f>TRIM(D25)=TRIM(IF(RIGHT(Sheet1!D25, 1) = ".", LEFT(Sheet1!D25, LEN(Sheet1!D25)-1),Sheet1!D25))</f>
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <f>TRIM(E25)=TRIM(IF(RIGHT(Sheet1!E25, 1) = ".", LEFT(Sheet1!E25, LEN(Sheet1!E25)-1),Sheet1!E25))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G26" t="b">
+        <f>TRIM(B26)=TRIM(IF(RIGHT(Sheet1!B26, 1) = ".", LEFT(Sheet1!B26, LEN(Sheet1!B26)-1),Sheet1!B26))</f>
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <f>TRIM(C26)=TRIM(IF(RIGHT(Sheet1!C26, 1) = ".", LEFT(Sheet1!C26, LEN(Sheet1!C26)-1),Sheet1!C26))</f>
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <f>TRIM(D26)=TRIM(IF(RIGHT(Sheet1!D26, 1) = ".", LEFT(Sheet1!D26, LEN(Sheet1!D26)-1),Sheet1!D26))</f>
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <f>TRIM(E26)=TRIM(IF(RIGHT(Sheet1!E26, 1) = ".", LEFT(Sheet1!E26, LEN(Sheet1!E26)-1),Sheet1!E26))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G27" t="b">
+        <f>TRIM(B27)=TRIM(IF(RIGHT(Sheet1!B27, 1) = ".", LEFT(Sheet1!B27, LEN(Sheet1!B27)-1),Sheet1!B27))</f>
+        <v>0</v>
+      </c>
+      <c r="H27" t="b">
+        <f>TRIM(C27)=TRIM(IF(RIGHT(Sheet1!C27, 1) = ".", LEFT(Sheet1!C27, LEN(Sheet1!C27)-1),Sheet1!C27))</f>
+        <v>0</v>
+      </c>
+      <c r="I27" t="b">
+        <f>TRIM(D27)=TRIM(IF(RIGHT(Sheet1!D27, 1) = ".", LEFT(Sheet1!D27, LEN(Sheet1!D27)-1),Sheet1!D27))</f>
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <f>TRIM(E27)=TRIM(IF(RIGHT(Sheet1!E27, 1) = ".", LEFT(Sheet1!E27, LEN(Sheet1!E27)-1),Sheet1!E27))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G28" t="b">
+        <f>TRIM(B28)=TRIM(IF(RIGHT(Sheet1!B28, 1) = ".", LEFT(Sheet1!B28, LEN(Sheet1!B28)-1),Sheet1!B28))</f>
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <f>TRIM(C28)=TRIM(IF(RIGHT(Sheet1!C28, 1) = ".", LEFT(Sheet1!C28, LEN(Sheet1!C28)-1),Sheet1!C28))</f>
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <f>TRIM(D28)=TRIM(IF(RIGHT(Sheet1!D28, 1) = ".", LEFT(Sheet1!D28, LEN(Sheet1!D28)-1),Sheet1!D28))</f>
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <f>TRIM(E28)=TRIM(IF(RIGHT(Sheet1!E28, 1) = ".", LEFT(Sheet1!E28, LEN(Sheet1!E28)-1),Sheet1!E28))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G29" t="b">
+        <f>TRIM(B29)=TRIM(IF(RIGHT(Sheet1!B29, 1) = ".", LEFT(Sheet1!B29, LEN(Sheet1!B29)-1),Sheet1!B29))</f>
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <f>TRIM(C29)=TRIM(IF(RIGHT(Sheet1!C29, 1) = ".", LEFT(Sheet1!C29, LEN(Sheet1!C29)-1),Sheet1!C29))</f>
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <f>TRIM(D29)=TRIM(IF(RIGHT(Sheet1!D29, 1) = ".", LEFT(Sheet1!D29, LEN(Sheet1!D29)-1),Sheet1!D29))</f>
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <f>TRIM(E29)=TRIM(IF(RIGHT(Sheet1!E29, 1) = ".", LEFT(Sheet1!E29, LEN(Sheet1!E29)-1),Sheet1!E29))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G30" t="b">
+        <f>TRIM(B30)=TRIM(IF(RIGHT(Sheet1!B30, 1) = ".", LEFT(Sheet1!B30, LEN(Sheet1!B30)-1),Sheet1!B30))</f>
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <f>TRIM(C30)=TRIM(IF(RIGHT(Sheet1!C30, 1) = ".", LEFT(Sheet1!C30, LEN(Sheet1!C30)-1),Sheet1!C30))</f>
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <f>TRIM(D30)=TRIM(IF(RIGHT(Sheet1!D30, 1) = ".", LEFT(Sheet1!D30, LEN(Sheet1!D30)-1),Sheet1!D30))</f>
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <f>TRIM(E30)=TRIM(IF(RIGHT(Sheet1!E30, 1) = ".", LEFT(Sheet1!E30, LEN(Sheet1!E30)-1),Sheet1!E30))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G31" t="b">
+        <f>TRIM(B31)=TRIM(IF(RIGHT(Sheet1!B31, 1) = ".", LEFT(Sheet1!B31, LEN(Sheet1!B31)-1),Sheet1!B31))</f>
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <f>TRIM(C31)=TRIM(IF(RIGHT(Sheet1!C31, 1) = ".", LEFT(Sheet1!C31, LEN(Sheet1!C31)-1),Sheet1!C31))</f>
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <f>TRIM(D31)=TRIM(IF(RIGHT(Sheet1!D31, 1) = ".", LEFT(Sheet1!D31, LEN(Sheet1!D31)-1),Sheet1!D31))</f>
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <f>TRIM(E31)=TRIM(IF(RIGHT(Sheet1!E31, 1) = ".", LEFT(Sheet1!E31, LEN(Sheet1!E31)-1),Sheet1!E31))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G32" t="b">
+        <f>TRIM(B32)=TRIM(IF(RIGHT(Sheet1!B32, 1) = ".", LEFT(Sheet1!B32, LEN(Sheet1!B32)-1),Sheet1!B32))</f>
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <f>TRIM(C32)=TRIM(IF(RIGHT(Sheet1!C32, 1) = ".", LEFT(Sheet1!C32, LEN(Sheet1!C32)-1),Sheet1!C32))</f>
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <f>TRIM(D32)=TRIM(IF(RIGHT(Sheet1!D32, 1) = ".", LEFT(Sheet1!D32, LEN(Sheet1!D32)-1),Sheet1!D32))</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <f>TRIM(E32)=TRIM(IF(RIGHT(Sheet1!E32, 1) = ".", LEFT(Sheet1!E32, LEN(Sheet1!E32)-1),Sheet1!E32))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" t="b">
+        <f>TRIM(B33)=TRIM(IF(RIGHT(Sheet1!B33, 1) = ".", LEFT(Sheet1!B33, LEN(Sheet1!B33)-1),Sheet1!B33))</f>
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <f>TRIM(C33)=TRIM(IF(RIGHT(Sheet1!C33, 1) = ".", LEFT(Sheet1!C33, LEN(Sheet1!C33)-1),Sheet1!C33))</f>
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
+        <f>TRIM(D33)=TRIM(IF(RIGHT(Sheet1!D33, 1) = ".", LEFT(Sheet1!D33, LEN(Sheet1!D33)-1),Sheet1!D33))</f>
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <f>TRIM(E33)=TRIM(IF(RIGHT(Sheet1!E33, 1) = ".", LEFT(Sheet1!E33, LEN(Sheet1!E33)-1),Sheet1!E33))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" t="b">
+        <f>TRIM(B34)=TRIM(IF(RIGHT(Sheet1!B34, 1) = ".", LEFT(Sheet1!B34, LEN(Sheet1!B34)-1),Sheet1!B34))</f>
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <f>TRIM(C34)=TRIM(IF(RIGHT(Sheet1!C34, 1) = ".", LEFT(Sheet1!C34, LEN(Sheet1!C34)-1),Sheet1!C34))</f>
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <f>TRIM(D34)=TRIM(IF(RIGHT(Sheet1!D34, 1) = ".", LEFT(Sheet1!D34, LEN(Sheet1!D34)-1),Sheet1!D34))</f>
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <f>TRIM(E34)=TRIM(IF(RIGHT(Sheet1!E34, 1) = ".", LEFT(Sheet1!E34, LEN(Sheet1!E34)-1),Sheet1!E34))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" t="b">
+        <f>TRIM(B35)=TRIM(IF(RIGHT(Sheet1!B35, 1) = ".", LEFT(Sheet1!B35, LEN(Sheet1!B35)-1),Sheet1!B35))</f>
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <f>TRIM(C35)=TRIM(IF(RIGHT(Sheet1!C35, 1) = ".", LEFT(Sheet1!C35, LEN(Sheet1!C35)-1),Sheet1!C35))</f>
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <f>TRIM(D35)=TRIM(IF(RIGHT(Sheet1!D35, 1) = ".", LEFT(Sheet1!D35, LEN(Sheet1!D35)-1),Sheet1!D35))</f>
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <f>TRIM(E35)=TRIM(IF(RIGHT(Sheet1!E35, 1) = ".", LEFT(Sheet1!E35, LEN(Sheet1!E35)-1),Sheet1!E35))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" t="b">
+        <f>TRIM(B36)=TRIM(IF(RIGHT(Sheet1!B36, 1) = ".", LEFT(Sheet1!B36, LEN(Sheet1!B36)-1),Sheet1!B36))</f>
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <f>TRIM(C36)=TRIM(IF(RIGHT(Sheet1!C36, 1) = ".", LEFT(Sheet1!C36, LEN(Sheet1!C36)-1),Sheet1!C36))</f>
+        <v>0</v>
+      </c>
+      <c r="I36" t="b">
+        <f>TRIM(D36)=TRIM(IF(RIGHT(Sheet1!D36, 1) = ".", LEFT(Sheet1!D36, LEN(Sheet1!D36)-1),Sheet1!D36))</f>
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <f>TRIM(E36)=TRIM(IF(RIGHT(Sheet1!E36, 1) = ".", LEFT(Sheet1!E36, LEN(Sheet1!E36)-1),Sheet1!E36))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G37" t="b">
+        <f>TRIM(B37)=TRIM(IF(RIGHT(Sheet1!B37, 1) = ".", LEFT(Sheet1!B37, LEN(Sheet1!B37)-1),Sheet1!B37))</f>
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <f>TRIM(C37)=TRIM(IF(RIGHT(Sheet1!C37, 1) = ".", LEFT(Sheet1!C37, LEN(Sheet1!C37)-1),Sheet1!C37))</f>
+        <v>0</v>
+      </c>
+      <c r="I37" t="b">
+        <f>TRIM(D37)=TRIM(IF(RIGHT(Sheet1!D37, 1) = ".", LEFT(Sheet1!D37, LEN(Sheet1!D37)-1),Sheet1!D37))</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <f>TRIM(E37)=TRIM(IF(RIGHT(Sheet1!E37, 1) = ".", LEFT(Sheet1!E37, LEN(Sheet1!E37)-1),Sheet1!E37))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G38" t="b">
+        <f>TRIM(B38)=TRIM(IF(RIGHT(Sheet1!B38, 1) = ".", LEFT(Sheet1!B38, LEN(Sheet1!B38)-1),Sheet1!B38))</f>
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <f>TRIM(C38)=TRIM(IF(RIGHT(Sheet1!C38, 1) = ".", LEFT(Sheet1!C38, LEN(Sheet1!C38)-1),Sheet1!C38))</f>
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <f>TRIM(D38)=TRIM(IF(RIGHT(Sheet1!D38, 1) = ".", LEFT(Sheet1!D38, LEN(Sheet1!D38)-1),Sheet1!D38))</f>
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <f>TRIM(E38)=TRIM(IF(RIGHT(Sheet1!E38, 1) = ".", LEFT(Sheet1!E38, LEN(Sheet1!E38)-1),Sheet1!E38))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G39" t="b">
+        <f>TRIM(B39)=TRIM(IF(RIGHT(Sheet1!B39, 1) = ".", LEFT(Sheet1!B39, LEN(Sheet1!B39)-1),Sheet1!B39))</f>
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <f>TRIM(C39)=TRIM(IF(RIGHT(Sheet1!C39, 1) = ".", LEFT(Sheet1!C39, LEN(Sheet1!C39)-1),Sheet1!C39))</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <f>TRIM(D39)=TRIM(IF(RIGHT(Sheet1!D39, 1) = ".", LEFT(Sheet1!D39, LEN(Sheet1!D39)-1),Sheet1!D39))</f>
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <f>TRIM(E39)=TRIM(IF(RIGHT(Sheet1!E39, 1) = ".", LEFT(Sheet1!E39, LEN(Sheet1!E39)-1),Sheet1!E39))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G40" t="b">
+        <f>TRIM(B40)=TRIM(IF(RIGHT(Sheet1!B40, 1) = ".", LEFT(Sheet1!B40, LEN(Sheet1!B40)-1),Sheet1!B40))</f>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <f>TRIM(C40)=TRIM(IF(RIGHT(Sheet1!C40, 1) = ".", LEFT(Sheet1!C40, LEN(Sheet1!C40)-1),Sheet1!C40))</f>
+        <v>0</v>
+      </c>
+      <c r="I40" t="b">
+        <f>TRIM(D40)=TRIM(IF(RIGHT(Sheet1!D40, 1) = ".", LEFT(Sheet1!D40, LEN(Sheet1!D40)-1),Sheet1!D40))</f>
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <f>TRIM(E40)=TRIM(IF(RIGHT(Sheet1!E40, 1) = ".", LEFT(Sheet1!E40, LEN(Sheet1!E40)-1),Sheet1!E40))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G41" t="b">
+        <f>TRIM(B41)=TRIM(IF(RIGHT(Sheet1!B41, 1) = ".", LEFT(Sheet1!B41, LEN(Sheet1!B41)-1),Sheet1!B41))</f>
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <f>TRIM(C41)=TRIM(IF(RIGHT(Sheet1!C41, 1) = ".", LEFT(Sheet1!C41, LEN(Sheet1!C41)-1),Sheet1!C41))</f>
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <f>TRIM(D41)=TRIM(IF(RIGHT(Sheet1!D41, 1) = ".", LEFT(Sheet1!D41, LEN(Sheet1!D41)-1),Sheet1!D41))</f>
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <f>TRIM(E41)=TRIM(IF(RIGHT(Sheet1!E41, 1) = ".", LEFT(Sheet1!E41, LEN(Sheet1!E41)-1),Sheet1!E41))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G42" t="b">
+        <f>TRIM(B42)=TRIM(IF(RIGHT(Sheet1!B42, 1) = ".", LEFT(Sheet1!B42, LEN(Sheet1!B42)-1),Sheet1!B42))</f>
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <f>TRIM(C42)=TRIM(IF(RIGHT(Sheet1!C42, 1) = ".", LEFT(Sheet1!C42, LEN(Sheet1!C42)-1),Sheet1!C42))</f>
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <f>TRIM(D42)=TRIM(IF(RIGHT(Sheet1!D42, 1) = ".", LEFT(Sheet1!D42, LEN(Sheet1!D42)-1),Sheet1!D42))</f>
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <f>TRIM(E42)=TRIM(IF(RIGHT(Sheet1!E42, 1) = ".", LEFT(Sheet1!E42, LEN(Sheet1!E42)-1),Sheet1!E42))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G43" t="b">
+        <f>TRIM(B43)=TRIM(IF(RIGHT(Sheet1!B43, 1) = ".", LEFT(Sheet1!B43, LEN(Sheet1!B43)-1),Sheet1!B43))</f>
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <f>TRIM(C43)=TRIM(IF(RIGHT(Sheet1!C43, 1) = ".", LEFT(Sheet1!C43, LEN(Sheet1!C43)-1),Sheet1!C43))</f>
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <f>TRIM(D43)=TRIM(IF(RIGHT(Sheet1!D43, 1) = ".", LEFT(Sheet1!D43, LEN(Sheet1!D43)-1),Sheet1!D43))</f>
+        <v>0</v>
+      </c>
+      <c r="J43" t="b">
+        <f>TRIM(E43)=TRIM(IF(RIGHT(Sheet1!E43, 1) = ".", LEFT(Sheet1!E43, LEN(Sheet1!E43)-1),Sheet1!E43))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G44" t="b">
+        <f>TRIM(B44)=TRIM(IF(RIGHT(Sheet1!B44, 1) = ".", LEFT(Sheet1!B44, LEN(Sheet1!B44)-1),Sheet1!B44))</f>
+        <v>0</v>
+      </c>
+      <c r="H44" t="b">
+        <f>TRIM(C44)=TRIM(IF(RIGHT(Sheet1!C44, 1) = ".", LEFT(Sheet1!C44, LEN(Sheet1!C44)-1),Sheet1!C44))</f>
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <f>TRIM(D44)=TRIM(IF(RIGHT(Sheet1!D44, 1) = ".", LEFT(Sheet1!D44, LEN(Sheet1!D44)-1),Sheet1!D44))</f>
+        <v>0</v>
+      </c>
+      <c r="J44" t="b">
+        <f>TRIM(E44)=TRIM(IF(RIGHT(Sheet1!E44, 1) = ".", LEFT(Sheet1!E44, LEN(Sheet1!E44)-1),Sheet1!E44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G45" t="b">
+        <f>TRIM(B45)=TRIM(IF(RIGHT(Sheet1!B45, 1) = ".", LEFT(Sheet1!B45, LEN(Sheet1!B45)-1),Sheet1!B45))</f>
+        <v>0</v>
+      </c>
+      <c r="H45" t="b">
+        <f>TRIM(C45)=TRIM(IF(RIGHT(Sheet1!C45, 1) = ".", LEFT(Sheet1!C45, LEN(Sheet1!C45)-1),Sheet1!C45))</f>
+        <v>0</v>
+      </c>
+      <c r="I45" t="b">
+        <f>TRIM(D45)=TRIM(IF(RIGHT(Sheet1!D45, 1) = ".", LEFT(Sheet1!D45, LEN(Sheet1!D45)-1),Sheet1!D45))</f>
+        <v>0</v>
+      </c>
+      <c r="J45" t="b">
+        <f>TRIM(E45)=TRIM(IF(RIGHT(Sheet1!E45, 1) = ".", LEFT(Sheet1!E45, LEN(Sheet1!E45)-1),Sheet1!E45))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G46" t="b">
+        <f>TRIM(B46)=TRIM(IF(RIGHT(Sheet1!B46, 1) = ".", LEFT(Sheet1!B46, LEN(Sheet1!B46)-1),Sheet1!B46))</f>
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <f>TRIM(C46)=TRIM(IF(RIGHT(Sheet1!C46, 1) = ".", LEFT(Sheet1!C46, LEN(Sheet1!C46)-1),Sheet1!C46))</f>
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <f>TRIM(D46)=TRIM(IF(RIGHT(Sheet1!D46, 1) = ".", LEFT(Sheet1!D46, LEN(Sheet1!D46)-1),Sheet1!D46))</f>
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <f>TRIM(E46)=TRIM(IF(RIGHT(Sheet1!E46, 1) = ".", LEFT(Sheet1!E46, LEN(Sheet1!E46)-1),Sheet1!E46))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G47" t="b">
+        <f>TRIM(B47)=TRIM(IF(RIGHT(Sheet1!B47, 1) = ".", LEFT(Sheet1!B47, LEN(Sheet1!B47)-1),Sheet1!B47))</f>
+        <v>0</v>
+      </c>
+      <c r="H47" t="b">
+        <f>TRIM(C47)=TRIM(IF(RIGHT(Sheet1!C47, 1) = ".", LEFT(Sheet1!C47, LEN(Sheet1!C47)-1),Sheet1!C47))</f>
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <f>TRIM(D47)=TRIM(IF(RIGHT(Sheet1!D47, 1) = ".", LEFT(Sheet1!D47, LEN(Sheet1!D47)-1),Sheet1!D47))</f>
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <f>TRIM(E47)=TRIM(IF(RIGHT(Sheet1!E47, 1) = ".", LEFT(Sheet1!E47, LEN(Sheet1!E47)-1),Sheet1!E47))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G48" t="b">
+        <f>TRIM(B48)=TRIM(IF(RIGHT(Sheet1!B48, 1) = ".", LEFT(Sheet1!B48, LEN(Sheet1!B48)-1),Sheet1!B48))</f>
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <f>TRIM(C48)=TRIM(IF(RIGHT(Sheet1!C48, 1) = ".", LEFT(Sheet1!C48, LEN(Sheet1!C48)-1),Sheet1!C48))</f>
+        <v>0</v>
+      </c>
+      <c r="I48" t="b">
+        <f>TRIM(D48)=TRIM(IF(RIGHT(Sheet1!D48, 1) = ".", LEFT(Sheet1!D48, LEN(Sheet1!D48)-1),Sheet1!D48))</f>
+        <v>0</v>
+      </c>
+      <c r="J48" t="b">
+        <f>TRIM(E48)=TRIM(IF(RIGHT(Sheet1!E48, 1) = ".", LEFT(Sheet1!E48, LEN(Sheet1!E48)-1),Sheet1!E48))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49" t="b">
+        <f>TRIM(B49)=TRIM(IF(RIGHT(Sheet1!B49, 1) = ".", LEFT(Sheet1!B49, LEN(Sheet1!B49)-1),Sheet1!B49))</f>
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <f>TRIM(C49)=TRIM(IF(RIGHT(Sheet1!C49, 1) = ".", LEFT(Sheet1!C49, LEN(Sheet1!C49)-1),Sheet1!C49))</f>
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <f>TRIM(D49)=TRIM(IF(RIGHT(Sheet1!D49, 1) = ".", LEFT(Sheet1!D49, LEN(Sheet1!D49)-1),Sheet1!D49))</f>
+        <v>0</v>
+      </c>
+      <c r="J49" t="b">
+        <f>TRIM(E49)=TRIM(IF(RIGHT(Sheet1!E49, 1) = ".", LEFT(Sheet1!E49, LEN(Sheet1!E49)-1),Sheet1!E49))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" t="b">
+        <f>TRIM(B50)=TRIM(IF(RIGHT(Sheet1!B50, 1) = ".", LEFT(Sheet1!B50, LEN(Sheet1!B50)-1),Sheet1!B50))</f>
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <f>TRIM(C50)=TRIM(IF(RIGHT(Sheet1!C50, 1) = ".", LEFT(Sheet1!C50, LEN(Sheet1!C50)-1),Sheet1!C50))</f>
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <f>TRIM(D50)=TRIM(IF(RIGHT(Sheet1!D50, 1) = ".", LEFT(Sheet1!D50, LEN(Sheet1!D50)-1),Sheet1!D50))</f>
+        <v>0</v>
+      </c>
+      <c r="J50" t="b">
+        <f>TRIM(E50)=TRIM(IF(RIGHT(Sheet1!E50, 1) = ".", LEFT(Sheet1!E50, LEN(Sheet1!E50)-1),Sheet1!E50))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G51" t="b">
+        <f>TRIM(B51)=TRIM(IF(RIGHT(Sheet1!B51, 1) = ".", LEFT(Sheet1!B51, LEN(Sheet1!B51)-1),Sheet1!B51))</f>
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <f>TRIM(C51)=TRIM(IF(RIGHT(Sheet1!C51, 1) = ".", LEFT(Sheet1!C51, LEN(Sheet1!C51)-1),Sheet1!C51))</f>
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <f>TRIM(D51)=TRIM(IF(RIGHT(Sheet1!D51, 1) = ".", LEFT(Sheet1!D51, LEN(Sheet1!D51)-1),Sheet1!D51))</f>
+        <v>0</v>
+      </c>
+      <c r="J51" t="b">
+        <f>TRIM(E51)=TRIM(IF(RIGHT(Sheet1!E51, 1) = ".", LEFT(Sheet1!E51, LEN(Sheet1!E51)-1),Sheet1!E51))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G52" t="b">
+        <f>TRIM(B52)=TRIM(IF(RIGHT(Sheet1!B52, 1) = ".", LEFT(Sheet1!B52, LEN(Sheet1!B52)-1),Sheet1!B52))</f>
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <f>TRIM(C52)=TRIM(IF(RIGHT(Sheet1!C52, 1) = ".", LEFT(Sheet1!C52, LEN(Sheet1!C52)-1),Sheet1!C52))</f>
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <f>TRIM(D52)=TRIM(IF(RIGHT(Sheet1!D52, 1) = ".", LEFT(Sheet1!D52, LEN(Sheet1!D52)-1),Sheet1!D52))</f>
+        <v>0</v>
+      </c>
+      <c r="J52" t="b">
+        <f>TRIM(E52)=TRIM(IF(RIGHT(Sheet1!E52, 1) = ".", LEFT(Sheet1!E52, LEN(Sheet1!E52)-1),Sheet1!E52))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G53" t="b">
+        <f>TRIM(B53)=TRIM(IF(RIGHT(Sheet1!B53, 1) = ".", LEFT(Sheet1!B53, LEN(Sheet1!B53)-1),Sheet1!B53))</f>
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <f>TRIM(C53)=TRIM(IF(RIGHT(Sheet1!C53, 1) = ".", LEFT(Sheet1!C53, LEN(Sheet1!C53)-1),Sheet1!C53))</f>
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <f>TRIM(D53)=TRIM(IF(RIGHT(Sheet1!D53, 1) = ".", LEFT(Sheet1!D53, LEN(Sheet1!D53)-1),Sheet1!D53))</f>
+        <v>0</v>
+      </c>
+      <c r="J53" t="b">
+        <f>TRIM(E53)=TRIM(IF(RIGHT(Sheet1!E53, 1) = ".", LEFT(Sheet1!E53, LEN(Sheet1!E53)-1),Sheet1!E53))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G54" t="b">
+        <f>TRIM(B54)=TRIM(IF(RIGHT(Sheet1!B54, 1) = ".", LEFT(Sheet1!B54, LEN(Sheet1!B54)-1),Sheet1!B54))</f>
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <f>TRIM(C54)=TRIM(IF(RIGHT(Sheet1!C54, 1) = ".", LEFT(Sheet1!C54, LEN(Sheet1!C54)-1),Sheet1!C54))</f>
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <f>TRIM(D54)=TRIM(IF(RIGHT(Sheet1!D54, 1) = ".", LEFT(Sheet1!D54, LEN(Sheet1!D54)-1),Sheet1!D54))</f>
+        <v>0</v>
+      </c>
+      <c r="J54" t="b">
+        <f>TRIM(E54)=TRIM(IF(RIGHT(Sheet1!E54, 1) = ".", LEFT(Sheet1!E54, LEN(Sheet1!E54)-1),Sheet1!E54))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G55" t="b">
+        <f>TRIM(B55)=TRIM(IF(RIGHT(Sheet1!B55, 1) = ".", LEFT(Sheet1!B55, LEN(Sheet1!B55)-1),Sheet1!B55))</f>
+        <v>0</v>
+      </c>
+      <c r="H55" t="b">
+        <f>TRIM(C55)=TRIM(IF(RIGHT(Sheet1!C55, 1) = ".", LEFT(Sheet1!C55, LEN(Sheet1!C55)-1),Sheet1!C55))</f>
+        <v>0</v>
+      </c>
+      <c r="I55" t="b">
+        <f>TRIM(D55)=TRIM(IF(RIGHT(Sheet1!D55, 1) = ".", LEFT(Sheet1!D55, LEN(Sheet1!D55)-1),Sheet1!D55))</f>
+        <v>0</v>
+      </c>
+      <c r="J55" t="b">
+        <f>TRIM(E55)=TRIM(IF(RIGHT(Sheet1!E55, 1) = ".", LEFT(Sheet1!E55, LEN(Sheet1!E55)-1),Sheet1!E55))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G56" t="b">
+        <f>TRIM(B56)=TRIM(IF(RIGHT(Sheet1!B56, 1) = ".", LEFT(Sheet1!B56, LEN(Sheet1!B56)-1),Sheet1!B56))</f>
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <f>TRIM(C56)=TRIM(IF(RIGHT(Sheet1!C56, 1) = ".", LEFT(Sheet1!C56, LEN(Sheet1!C56)-1),Sheet1!C56))</f>
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <f>TRIM(D56)=TRIM(IF(RIGHT(Sheet1!D56, 1) = ".", LEFT(Sheet1!D56, LEN(Sheet1!D56)-1),Sheet1!D56))</f>
+        <v>0</v>
+      </c>
+      <c r="J56" t="b">
+        <f>TRIM(E56)=TRIM(IF(RIGHT(Sheet1!E56, 1) = ".", LEFT(Sheet1!E56, LEN(Sheet1!E56)-1),Sheet1!E56))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G57" t="b">
+        <f>TRIM(B57)=TRIM(IF(RIGHT(Sheet1!B57, 1) = ".", LEFT(Sheet1!B57, LEN(Sheet1!B57)-1),Sheet1!B57))</f>
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <f>TRIM(C57)=TRIM(IF(RIGHT(Sheet1!C57, 1) = ".", LEFT(Sheet1!C57, LEN(Sheet1!C57)-1),Sheet1!C57))</f>
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <f>TRIM(D57)=TRIM(IF(RIGHT(Sheet1!D57, 1) = ".", LEFT(Sheet1!D57, LEN(Sheet1!D57)-1),Sheet1!D57))</f>
+        <v>0</v>
+      </c>
+      <c r="J57" t="b">
+        <f>TRIM(E57)=TRIM(IF(RIGHT(Sheet1!E57, 1) = ".", LEFT(Sheet1!E57, LEN(Sheet1!E57)-1),Sheet1!E57))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G58" t="b">
+        <f>TRIM(B58)=TRIM(IF(RIGHT(Sheet1!B58, 1) = ".", LEFT(Sheet1!B58, LEN(Sheet1!B58)-1),Sheet1!B58))</f>
+        <v>0</v>
+      </c>
+      <c r="H58" t="b">
+        <f>TRIM(C58)=TRIM(IF(RIGHT(Sheet1!C58, 1) = ".", LEFT(Sheet1!C58, LEN(Sheet1!C58)-1),Sheet1!C58))</f>
+        <v>0</v>
+      </c>
+      <c r="I58" t="b">
+        <f>TRIM(D58)=TRIM(IF(RIGHT(Sheet1!D58, 1) = ".", LEFT(Sheet1!D58, LEN(Sheet1!D58)-1),Sheet1!D58))</f>
+        <v>0</v>
+      </c>
+      <c r="J58" t="b">
+        <f>TRIM(E58)=TRIM(IF(RIGHT(Sheet1!E58, 1) = ".", LEFT(Sheet1!E58, LEN(Sheet1!E58)-1),Sheet1!E58))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G59" t="b">
+        <f>TRIM(B59)=TRIM(IF(RIGHT(Sheet1!B59, 1) = ".", LEFT(Sheet1!B59, LEN(Sheet1!B59)-1),Sheet1!B59))</f>
+        <v>0</v>
+      </c>
+      <c r="H59" t="b">
+        <f>TRIM(C59)=TRIM(IF(RIGHT(Sheet1!C59, 1) = ".", LEFT(Sheet1!C59, LEN(Sheet1!C59)-1),Sheet1!C59))</f>
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <f>TRIM(D59)=TRIM(IF(RIGHT(Sheet1!D59, 1) = ".", LEFT(Sheet1!D59, LEN(Sheet1!D59)-1),Sheet1!D59))</f>
+        <v>0</v>
+      </c>
+      <c r="J59" t="b">
+        <f>TRIM(E59)=TRIM(IF(RIGHT(Sheet1!E59, 1) = ".", LEFT(Sheet1!E59, LEN(Sheet1!E59)-1),Sheet1!E59))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G60" t="b">
+        <f>TRIM(B60)=TRIM(IF(RIGHT(Sheet1!B60, 1) = ".", LEFT(Sheet1!B60, LEN(Sheet1!B60)-1),Sheet1!B60))</f>
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <f>TRIM(C60)=TRIM(IF(RIGHT(Sheet1!C60, 1) = ".", LEFT(Sheet1!C60, LEN(Sheet1!C60)-1),Sheet1!C60))</f>
+        <v>0</v>
+      </c>
+      <c r="I60" t="b">
+        <f>TRIM(D60)=TRIM(IF(RIGHT(Sheet1!D60, 1) = ".", LEFT(Sheet1!D60, LEN(Sheet1!D60)-1),Sheet1!D60))</f>
+        <v>0</v>
+      </c>
+      <c r="J60" t="b">
+        <f>TRIM(E60)=TRIM(IF(RIGHT(Sheet1!E60, 1) = ".", LEFT(Sheet1!E60, LEN(Sheet1!E60)-1),Sheet1!E60))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G61" t="b">
+        <f>TRIM(B61)=TRIM(IF(RIGHT(Sheet1!B61, 1) = ".", LEFT(Sheet1!B61, LEN(Sheet1!B61)-1),Sheet1!B61))</f>
+        <v>0</v>
+      </c>
+      <c r="H61" t="b">
+        <f>TRIM(C61)=TRIM(IF(RIGHT(Sheet1!C61, 1) = ".", LEFT(Sheet1!C61, LEN(Sheet1!C61)-1),Sheet1!C61))</f>
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <f>TRIM(D61)=TRIM(IF(RIGHT(Sheet1!D61, 1) = ".", LEFT(Sheet1!D61, LEN(Sheet1!D61)-1),Sheet1!D61))</f>
+        <v>0</v>
+      </c>
+      <c r="J61" t="b">
+        <f>TRIM(E61)=TRIM(IF(RIGHT(Sheet1!E61, 1) = ".", LEFT(Sheet1!E61, LEN(Sheet1!E61)-1),Sheet1!E61))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G62" t="b">
+        <f>TRIM(B62)=TRIM(IF(RIGHT(Sheet1!B62, 1) = ".", LEFT(Sheet1!B62, LEN(Sheet1!B62)-1),Sheet1!B62))</f>
+        <v>0</v>
+      </c>
+      <c r="H62" t="b">
+        <f>TRIM(C62)=TRIM(IF(RIGHT(Sheet1!C62, 1) = ".", LEFT(Sheet1!C62, LEN(Sheet1!C62)-1),Sheet1!C62))</f>
+        <v>0</v>
+      </c>
+      <c r="I62" t="b">
+        <f>TRIM(D62)=TRIM(IF(RIGHT(Sheet1!D62, 1) = ".", LEFT(Sheet1!D62, LEN(Sheet1!D62)-1),Sheet1!D62))</f>
+        <v>0</v>
+      </c>
+      <c r="J62" t="b">
+        <f>TRIM(E62)=TRIM(IF(RIGHT(Sheet1!E62, 1) = ".", LEFT(Sheet1!E62, LEN(Sheet1!E62)-1),Sheet1!E62))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G63" t="b">
+        <f>TRIM(B63)=TRIM(IF(RIGHT(Sheet1!B63, 1) = ".", LEFT(Sheet1!B63, LEN(Sheet1!B63)-1),Sheet1!B63))</f>
+        <v>0</v>
+      </c>
+      <c r="H63" t="b">
+        <f>TRIM(C63)=TRIM(IF(RIGHT(Sheet1!C63, 1) = ".", LEFT(Sheet1!C63, LEN(Sheet1!C63)-1),Sheet1!C63))</f>
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <f>TRIM(D63)=TRIM(IF(RIGHT(Sheet1!D63, 1) = ".", LEFT(Sheet1!D63, LEN(Sheet1!D63)-1),Sheet1!D63))</f>
+        <v>0</v>
+      </c>
+      <c r="J63" t="b">
+        <f>TRIM(E63)=TRIM(IF(RIGHT(Sheet1!E63, 1) = ".", LEFT(Sheet1!E63, LEN(Sheet1!E63)-1),Sheet1!E63))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G64" t="b">
+        <f>TRIM(B64)=TRIM(IF(RIGHT(Sheet1!B64, 1) = ".", LEFT(Sheet1!B64, LEN(Sheet1!B64)-1),Sheet1!B64))</f>
+        <v>0</v>
+      </c>
+      <c r="H64" t="b">
+        <f>TRIM(C64)=TRIM(IF(RIGHT(Sheet1!C64, 1) = ".", LEFT(Sheet1!C64, LEN(Sheet1!C64)-1),Sheet1!C64))</f>
+        <v>0</v>
+      </c>
+      <c r="I64" t="b">
+        <f>TRIM(D64)=TRIM(IF(RIGHT(Sheet1!D64, 1) = ".", LEFT(Sheet1!D64, LEN(Sheet1!D64)-1),Sheet1!D64))</f>
+        <v>0</v>
+      </c>
+      <c r="J64" t="b">
+        <f>TRIM(E64)=TRIM(IF(RIGHT(Sheet1!E64, 1) = ".", LEFT(Sheet1!E64, LEN(Sheet1!E64)-1),Sheet1!E64))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G65" t="b">
+        <f>TRIM(B65)=TRIM(IF(RIGHT(Sheet1!B65, 1) = ".", LEFT(Sheet1!B65, LEN(Sheet1!B65)-1),Sheet1!B65))</f>
+        <v>0</v>
+      </c>
+      <c r="H65" t="b">
+        <f>TRIM(C65)=TRIM(IF(RIGHT(Sheet1!C65, 1) = ".", LEFT(Sheet1!C65, LEN(Sheet1!C65)-1),Sheet1!C65))</f>
+        <v>0</v>
+      </c>
+      <c r="I65" t="b">
+        <f>TRIM(D65)=TRIM(IF(RIGHT(Sheet1!D65, 1) = ".", LEFT(Sheet1!D65, LEN(Sheet1!D65)-1),Sheet1!D65))</f>
+        <v>0</v>
+      </c>
+      <c r="J65" t="b">
+        <f>TRIM(E65)=TRIM(IF(RIGHT(Sheet1!E65, 1) = ".", LEFT(Sheet1!E65, LEN(Sheet1!E65)-1),Sheet1!E65))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G66" t="b">
+        <f>TRIM(B66)=TRIM(IF(RIGHT(Sheet1!B66, 1) = ".", LEFT(Sheet1!B66, LEN(Sheet1!B66)-1),Sheet1!B66))</f>
+        <v>0</v>
+      </c>
+      <c r="H66" t="b">
+        <f>TRIM(C66)=TRIM(IF(RIGHT(Sheet1!C66, 1) = ".", LEFT(Sheet1!C66, LEN(Sheet1!C66)-1),Sheet1!C66))</f>
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <f>TRIM(D66)=TRIM(IF(RIGHT(Sheet1!D66, 1) = ".", LEFT(Sheet1!D66, LEN(Sheet1!D66)-1),Sheet1!D66))</f>
+        <v>0</v>
+      </c>
+      <c r="J66" t="b">
+        <f>TRIM(E66)=TRIM(IF(RIGHT(Sheet1!E66, 1) = ".", LEFT(Sheet1!E66, LEN(Sheet1!E66)-1),Sheet1!E66))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G67" t="b">
+        <f>TRIM(B67)=TRIM(IF(RIGHT(Sheet1!B67, 1) = ".", LEFT(Sheet1!B67, LEN(Sheet1!B67)-1),Sheet1!B67))</f>
+        <v>0</v>
+      </c>
+      <c r="H67" t="b">
+        <f>TRIM(C67)=TRIM(IF(RIGHT(Sheet1!C67, 1) = ".", LEFT(Sheet1!C67, LEN(Sheet1!C67)-1),Sheet1!C67))</f>
+        <v>0</v>
+      </c>
+      <c r="I67" t="b">
+        <f>TRIM(D67)=TRIM(IF(RIGHT(Sheet1!D67, 1) = ".", LEFT(Sheet1!D67, LEN(Sheet1!D67)-1),Sheet1!D67))</f>
+        <v>0</v>
+      </c>
+      <c r="J67" t="b">
+        <f>TRIM(E67)=TRIM(IF(RIGHT(Sheet1!E67, 1) = ".", LEFT(Sheet1!E67, LEN(Sheet1!E67)-1),Sheet1!E67))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G68" t="b">
+        <f>TRIM(B68)=TRIM(IF(RIGHT(Sheet1!B68, 1) = ".", LEFT(Sheet1!B68, LEN(Sheet1!B68)-1),Sheet1!B68))</f>
+        <v>0</v>
+      </c>
+      <c r="H68" t="b">
+        <f>TRIM(C68)=TRIM(IF(RIGHT(Sheet1!C68, 1) = ".", LEFT(Sheet1!C68, LEN(Sheet1!C68)-1),Sheet1!C68))</f>
+        <v>0</v>
+      </c>
+      <c r="I68" t="b">
+        <f>TRIM(D68)=TRIM(IF(RIGHT(Sheet1!D68, 1) = ".", LEFT(Sheet1!D68, LEN(Sheet1!D68)-1),Sheet1!D68))</f>
+        <v>0</v>
+      </c>
+      <c r="J68" t="b">
+        <f>TRIM(E68)=TRIM(IF(RIGHT(Sheet1!E68, 1) = ".", LEFT(Sheet1!E68, LEN(Sheet1!E68)-1),Sheet1!E68))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G69" t="b">
+        <f>TRIM(B69)=TRIM(IF(RIGHT(Sheet1!B69, 1) = ".", LEFT(Sheet1!B69, LEN(Sheet1!B69)-1),Sheet1!B69))</f>
+        <v>0</v>
+      </c>
+      <c r="H69" t="b">
+        <f>TRIM(C69)=TRIM(IF(RIGHT(Sheet1!C69, 1) = ".", LEFT(Sheet1!C69, LEN(Sheet1!C69)-1),Sheet1!C69))</f>
+        <v>0</v>
+      </c>
+      <c r="I69" t="b">
+        <f>TRIM(D69)=TRIM(IF(RIGHT(Sheet1!D69, 1) = ".", LEFT(Sheet1!D69, LEN(Sheet1!D69)-1),Sheet1!D69))</f>
+        <v>0</v>
+      </c>
+      <c r="J69" t="b">
+        <f>TRIM(E69)=TRIM(IF(RIGHT(Sheet1!E69, 1) = ".", LEFT(Sheet1!E69, LEN(Sheet1!E69)-1),Sheet1!E69))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G70" t="b">
+        <f>TRIM(B70)=TRIM(IF(RIGHT(Sheet1!B70, 1) = ".", LEFT(Sheet1!B70, LEN(Sheet1!B70)-1),Sheet1!B70))</f>
+        <v>0</v>
+      </c>
+      <c r="H70" t="b">
+        <f>TRIM(C70)=TRIM(IF(RIGHT(Sheet1!C70, 1) = ".", LEFT(Sheet1!C70, LEN(Sheet1!C70)-1),Sheet1!C70))</f>
+        <v>0</v>
+      </c>
+      <c r="I70" t="b">
+        <f>TRIM(D70)=TRIM(IF(RIGHT(Sheet1!D70, 1) = ".", LEFT(Sheet1!D70, LEN(Sheet1!D70)-1),Sheet1!D70))</f>
+        <v>0</v>
+      </c>
+      <c r="J70" t="b">
+        <f>TRIM(E70)=TRIM(IF(RIGHT(Sheet1!E70, 1) = ".", LEFT(Sheet1!E70, LEN(Sheet1!E70)-1),Sheet1!E70))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G71" t="b">
+        <f>TRIM(B71)=TRIM(IF(RIGHT(Sheet1!B71, 1) = ".", LEFT(Sheet1!B71, LEN(Sheet1!B71)-1),Sheet1!B71))</f>
+        <v>0</v>
+      </c>
+      <c r="H71" t="b">
+        <f>TRIM(C71)=TRIM(IF(RIGHT(Sheet1!C71, 1) = ".", LEFT(Sheet1!C71, LEN(Sheet1!C71)-1),Sheet1!C71))</f>
+        <v>0</v>
+      </c>
+      <c r="I71" t="b">
+        <f>TRIM(D71)=TRIM(IF(RIGHT(Sheet1!D71, 1) = ".", LEFT(Sheet1!D71, LEN(Sheet1!D71)-1),Sheet1!D71))</f>
+        <v>0</v>
+      </c>
+      <c r="J71" t="b">
+        <f>TRIM(E71)=TRIM(IF(RIGHT(Sheet1!E71, 1) = ".", LEFT(Sheet1!E71, LEN(Sheet1!E71)-1),Sheet1!E71))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G72" t="b">
+        <f>TRIM(B72)=TRIM(IF(RIGHT(Sheet1!B72, 1) = ".", LEFT(Sheet1!B72, LEN(Sheet1!B72)-1),Sheet1!B72))</f>
+        <v>0</v>
+      </c>
+      <c r="H72" t="b">
+        <f>TRIM(C72)=TRIM(IF(RIGHT(Sheet1!C72, 1) = ".", LEFT(Sheet1!C72, LEN(Sheet1!C72)-1),Sheet1!C72))</f>
+        <v>0</v>
+      </c>
+      <c r="I72" t="b">
+        <f>TRIM(D72)=TRIM(IF(RIGHT(Sheet1!D72, 1) = ".", LEFT(Sheet1!D72, LEN(Sheet1!D72)-1),Sheet1!D72))</f>
+        <v>0</v>
+      </c>
+      <c r="J72" t="b">
+        <f>TRIM(E72)=TRIM(IF(RIGHT(Sheet1!E72, 1) = ".", LEFT(Sheet1!E72, LEN(Sheet1!E72)-1),Sheet1!E72))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G73" t="b">
+        <f>TRIM(B73)=TRIM(IF(RIGHT(Sheet1!B73, 1) = ".", LEFT(Sheet1!B73, LEN(Sheet1!B73)-1),Sheet1!B73))</f>
+        <v>0</v>
+      </c>
+      <c r="H73" t="b">
+        <f>TRIM(C73)=TRIM(IF(RIGHT(Sheet1!C73, 1) = ".", LEFT(Sheet1!C73, LEN(Sheet1!C73)-1),Sheet1!C73))</f>
+        <v>0</v>
+      </c>
+      <c r="I73" t="b">
+        <f>TRIM(D73)=TRIM(IF(RIGHT(Sheet1!D73, 1) = ".", LEFT(Sheet1!D73, LEN(Sheet1!D73)-1),Sheet1!D73))</f>
+        <v>0</v>
+      </c>
+      <c r="J73" t="b">
+        <f>TRIM(E73)=TRIM(IF(RIGHT(Sheet1!E73, 1) = ".", LEFT(Sheet1!E73, LEN(Sheet1!E73)-1),Sheet1!E73))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G74" t="b">
+        <f>TRIM(B74)=TRIM(IF(RIGHT(Sheet1!B74, 1) = ".", LEFT(Sheet1!B74, LEN(Sheet1!B74)-1),Sheet1!B74))</f>
+        <v>0</v>
+      </c>
+      <c r="H74" t="b">
+        <f>TRIM(C74)=TRIM(IF(RIGHT(Sheet1!C74, 1) = ".", LEFT(Sheet1!C74, LEN(Sheet1!C74)-1),Sheet1!C74))</f>
+        <v>0</v>
+      </c>
+      <c r="I74" t="b">
+        <f>TRIM(D74)=TRIM(IF(RIGHT(Sheet1!D74, 1) = ".", LEFT(Sheet1!D74, LEN(Sheet1!D74)-1),Sheet1!D74))</f>
+        <v>0</v>
+      </c>
+      <c r="J74" t="b">
+        <f>TRIM(E74)=TRIM(IF(RIGHT(Sheet1!E74, 1) = ".", LEFT(Sheet1!E74, LEN(Sheet1!E74)-1),Sheet1!E74))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G75" t="b">
+        <f>TRIM(B75)=TRIM(IF(RIGHT(Sheet1!B75, 1) = ".", LEFT(Sheet1!B75, LEN(Sheet1!B75)-1),Sheet1!B75))</f>
+        <v>0</v>
+      </c>
+      <c r="H75" t="b">
+        <f>TRIM(C75)=TRIM(IF(RIGHT(Sheet1!C75, 1) = ".", LEFT(Sheet1!C75, LEN(Sheet1!C75)-1),Sheet1!C75))</f>
+        <v>0</v>
+      </c>
+      <c r="I75" t="b">
+        <f>TRIM(D75)=TRIM(IF(RIGHT(Sheet1!D75, 1) = ".", LEFT(Sheet1!D75, LEN(Sheet1!D75)-1),Sheet1!D75))</f>
+        <v>0</v>
+      </c>
+      <c r="J75" t="b">
+        <f>TRIM(E75)=TRIM(IF(RIGHT(Sheet1!E75, 1) = ".", LEFT(Sheet1!E75, LEN(Sheet1!E75)-1),Sheet1!E75))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G76" t="b">
+        <f>TRIM(B76)=TRIM(IF(RIGHT(Sheet1!B76, 1) = ".", LEFT(Sheet1!B76, LEN(Sheet1!B76)-1),Sheet1!B76))</f>
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <f>TRIM(C76)=TRIM(IF(RIGHT(Sheet1!C76, 1) = ".", LEFT(Sheet1!C76, LEN(Sheet1!C76)-1),Sheet1!C76))</f>
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <f>TRIM(D76)=TRIM(IF(RIGHT(Sheet1!D76, 1) = ".", LEFT(Sheet1!D76, LEN(Sheet1!D76)-1),Sheet1!D76))</f>
+        <v>0</v>
+      </c>
+      <c r="J76" t="b">
+        <f>TRIM(E76)=TRIM(IF(RIGHT(Sheet1!E76, 1) = ".", LEFT(Sheet1!E76, LEN(Sheet1!E76)-1),Sheet1!E76))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G77" t="b">
+        <f>TRIM(B77)=TRIM(IF(RIGHT(Sheet1!B77, 1) = ".", LEFT(Sheet1!B77, LEN(Sheet1!B77)-1),Sheet1!B77))</f>
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <f>TRIM(C77)=TRIM(IF(RIGHT(Sheet1!C77, 1) = ".", LEFT(Sheet1!C77, LEN(Sheet1!C77)-1),Sheet1!C77))</f>
+        <v>0</v>
+      </c>
+      <c r="I77" t="b">
+        <f>TRIM(D77)=TRIM(IF(RIGHT(Sheet1!D77, 1) = ".", LEFT(Sheet1!D77, LEN(Sheet1!D77)-1),Sheet1!D77))</f>
+        <v>0</v>
+      </c>
+      <c r="J77" t="b">
+        <f>TRIM(E77)=TRIM(IF(RIGHT(Sheet1!E77, 1) = ".", LEFT(Sheet1!E77, LEN(Sheet1!E77)-1),Sheet1!E77))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G78" t="b">
+        <f>TRIM(B78)=TRIM(IF(RIGHT(Sheet1!B78, 1) = ".", LEFT(Sheet1!B78, LEN(Sheet1!B78)-1),Sheet1!B78))</f>
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <f>TRIM(C78)=TRIM(IF(RIGHT(Sheet1!C78, 1) = ".", LEFT(Sheet1!C78, LEN(Sheet1!C78)-1),Sheet1!C78))</f>
+        <v>0</v>
+      </c>
+      <c r="I78" t="b">
+        <f>TRIM(D78)=TRIM(IF(RIGHT(Sheet1!D78, 1) = ".", LEFT(Sheet1!D78, LEN(Sheet1!D78)-1),Sheet1!D78))</f>
+        <v>0</v>
+      </c>
+      <c r="J78" t="b">
+        <f>TRIM(E78)=TRIM(IF(RIGHT(Sheet1!E78, 1) = ".", LEFT(Sheet1!E78, LEN(Sheet1!E78)-1),Sheet1!E78))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G79" t="b">
+        <f>TRIM(B79)=TRIM(IF(RIGHT(Sheet1!B79, 1) = ".", LEFT(Sheet1!B79, LEN(Sheet1!B79)-1),Sheet1!B79))</f>
+        <v>0</v>
+      </c>
+      <c r="H79" t="b">
+        <f>TRIM(C79)=TRIM(IF(RIGHT(Sheet1!C79, 1) = ".", LEFT(Sheet1!C79, LEN(Sheet1!C79)-1),Sheet1!C79))</f>
+        <v>0</v>
+      </c>
+      <c r="I79" t="b">
+        <f>TRIM(D79)=TRIM(IF(RIGHT(Sheet1!D79, 1) = ".", LEFT(Sheet1!D79, LEN(Sheet1!D79)-1),Sheet1!D79))</f>
+        <v>0</v>
+      </c>
+      <c r="J79" t="b">
+        <f>TRIM(E79)=TRIM(IF(RIGHT(Sheet1!E79, 1) = ".", LEFT(Sheet1!E79, LEN(Sheet1!E79)-1),Sheet1!E79))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G80" t="b">
+        <f>TRIM(B80)=TRIM(IF(RIGHT(Sheet1!B80, 1) = ".", LEFT(Sheet1!B80, LEN(Sheet1!B80)-1),Sheet1!B80))</f>
+        <v>0</v>
+      </c>
+      <c r="H80" t="b">
+        <f>TRIM(C80)=TRIM(IF(RIGHT(Sheet1!C80, 1) = ".", LEFT(Sheet1!C80, LEN(Sheet1!C80)-1),Sheet1!C80))</f>
+        <v>0</v>
+      </c>
+      <c r="I80" t="b">
+        <f>TRIM(D80)=TRIM(IF(RIGHT(Sheet1!D80, 1) = ".", LEFT(Sheet1!D80, LEN(Sheet1!D80)-1),Sheet1!D80))</f>
+        <v>0</v>
+      </c>
+      <c r="J80" t="b">
+        <f>TRIM(E80)=TRIM(IF(RIGHT(Sheet1!E80, 1) = ".", LEFT(Sheet1!E80, LEN(Sheet1!E80)-1),Sheet1!E80))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G81" t="b">
+        <f>TRIM(B81)=TRIM(IF(RIGHT(Sheet1!B81, 1) = ".", LEFT(Sheet1!B81, LEN(Sheet1!B81)-1),Sheet1!B81))</f>
+        <v>0</v>
+      </c>
+      <c r="H81" t="b">
+        <f>TRIM(C81)=TRIM(IF(RIGHT(Sheet1!C81, 1) = ".", LEFT(Sheet1!C81, LEN(Sheet1!C81)-1),Sheet1!C81))</f>
+        <v>0</v>
+      </c>
+      <c r="I81" t="b">
+        <f>TRIM(D81)=TRIM(IF(RIGHT(Sheet1!D81, 1) = ".", LEFT(Sheet1!D81, LEN(Sheet1!D81)-1),Sheet1!D81))</f>
+        <v>0</v>
+      </c>
+      <c r="J81" t="b">
+        <f>TRIM(E81)=TRIM(IF(RIGHT(Sheet1!E81, 1) = ".", LEFT(Sheet1!E81, LEN(Sheet1!E81)-1),Sheet1!E81))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G82" t="b">
+        <f>TRIM(B82)=TRIM(IF(RIGHT(Sheet1!B82, 1) = ".", LEFT(Sheet1!B82, LEN(Sheet1!B82)-1),Sheet1!B82))</f>
+        <v>0</v>
+      </c>
+      <c r="H82" t="b">
+        <f>TRIM(C82)=TRIM(IF(RIGHT(Sheet1!C82, 1) = ".", LEFT(Sheet1!C82, LEN(Sheet1!C82)-1),Sheet1!C82))</f>
+        <v>0</v>
+      </c>
+      <c r="I82" t="b">
+        <f>TRIM(D82)=TRIM(IF(RIGHT(Sheet1!D82, 1) = ".", LEFT(Sheet1!D82, LEN(Sheet1!D82)-1),Sheet1!D82))</f>
+        <v>0</v>
+      </c>
+      <c r="J82" t="b">
+        <f>TRIM(E82)=TRIM(IF(RIGHT(Sheet1!E82, 1) = ".", LEFT(Sheet1!E82, LEN(Sheet1!E82)-1),Sheet1!E82))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G83" t="b">
+        <f>TRIM(B83)=TRIM(IF(RIGHT(Sheet1!B83, 1) = ".", LEFT(Sheet1!B83, LEN(Sheet1!B83)-1),Sheet1!B83))</f>
+        <v>0</v>
+      </c>
+      <c r="H83" t="b">
+        <f>TRIM(C83)=TRIM(IF(RIGHT(Sheet1!C83, 1) = ".", LEFT(Sheet1!C83, LEN(Sheet1!C83)-1),Sheet1!C83))</f>
+        <v>0</v>
+      </c>
+      <c r="I83" t="b">
+        <f>TRIM(D83)=TRIM(IF(RIGHT(Sheet1!D83, 1) = ".", LEFT(Sheet1!D83, LEN(Sheet1!D83)-1),Sheet1!D83))</f>
+        <v>0</v>
+      </c>
+      <c r="J83" t="b">
+        <f>TRIM(E83)=TRIM(IF(RIGHT(Sheet1!E83, 1) = ".", LEFT(Sheet1!E83, LEN(Sheet1!E83)-1),Sheet1!E83))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G84" t="b">
+        <f>TRIM(B84)=TRIM(IF(RIGHT(Sheet1!B84, 1) = ".", LEFT(Sheet1!B84, LEN(Sheet1!B84)-1),Sheet1!B84))</f>
+        <v>0</v>
+      </c>
+      <c r="H84" t="b">
+        <f>TRIM(C84)=TRIM(IF(RIGHT(Sheet1!C84, 1) = ".", LEFT(Sheet1!C84, LEN(Sheet1!C84)-1),Sheet1!C84))</f>
+        <v>0</v>
+      </c>
+      <c r="I84" t="b">
+        <f>TRIM(D84)=TRIM(IF(RIGHT(Sheet1!D84, 1) = ".", LEFT(Sheet1!D84, LEN(Sheet1!D84)-1),Sheet1!D84))</f>
+        <v>0</v>
+      </c>
+      <c r="J84" t="b">
+        <f>TRIM(E84)=TRIM(IF(RIGHT(Sheet1!E84, 1) = ".", LEFT(Sheet1!E84, LEN(Sheet1!E84)-1),Sheet1!E84))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G85" t="b">
+        <f>TRIM(B85)=TRIM(IF(RIGHT(Sheet1!B85, 1) = ".", LEFT(Sheet1!B85, LEN(Sheet1!B85)-1),Sheet1!B85))</f>
+        <v>0</v>
+      </c>
+      <c r="H85" t="b">
+        <f>TRIM(C85)=TRIM(IF(RIGHT(Sheet1!C85, 1) = ".", LEFT(Sheet1!C85, LEN(Sheet1!C85)-1),Sheet1!C85))</f>
+        <v>0</v>
+      </c>
+      <c r="I85" t="b">
+        <f>TRIM(D85)=TRIM(IF(RIGHT(Sheet1!D85, 1) = ".", LEFT(Sheet1!D85, LEN(Sheet1!D85)-1),Sheet1!D85))</f>
+        <v>0</v>
+      </c>
+      <c r="J85" t="b">
+        <f>TRIM(E85)=TRIM(IF(RIGHT(Sheet1!E85, 1) = ".", LEFT(Sheet1!E85, LEN(Sheet1!E85)-1),Sheet1!E85))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G86" t="b">
+        <f>TRIM(B86)=TRIM(IF(RIGHT(Sheet1!B86, 1) = ".", LEFT(Sheet1!B86, LEN(Sheet1!B86)-1),Sheet1!B86))</f>
+        <v>0</v>
+      </c>
+      <c r="H86" t="b">
+        <f>TRIM(C86)=TRIM(IF(RIGHT(Sheet1!C86, 1) = ".", LEFT(Sheet1!C86, LEN(Sheet1!C86)-1),Sheet1!C86))</f>
+        <v>0</v>
+      </c>
+      <c r="I86" t="b">
+        <f>TRIM(D86)=TRIM(IF(RIGHT(Sheet1!D86, 1) = ".", LEFT(Sheet1!D86, LEN(Sheet1!D86)-1),Sheet1!D86))</f>
+        <v>0</v>
+      </c>
+      <c r="J86" t="b">
+        <f>TRIM(E86)=TRIM(IF(RIGHT(Sheet1!E86, 1) = ".", LEFT(Sheet1!E86, LEN(Sheet1!E86)-1),Sheet1!E86))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G87" t="b">
+        <f>TRIM(B87)=TRIM(IF(RIGHT(Sheet1!B87, 1) = ".", LEFT(Sheet1!B87, LEN(Sheet1!B87)-1),Sheet1!B87))</f>
+        <v>0</v>
+      </c>
+      <c r="H87" t="b">
+        <f>TRIM(C87)=TRIM(IF(RIGHT(Sheet1!C87, 1) = ".", LEFT(Sheet1!C87, LEN(Sheet1!C87)-1),Sheet1!C87))</f>
+        <v>0</v>
+      </c>
+      <c r="I87" t="b">
+        <f>TRIM(D87)=TRIM(IF(RIGHT(Sheet1!D87, 1) = ".", LEFT(Sheet1!D87, LEN(Sheet1!D87)-1),Sheet1!D87))</f>
+        <v>0</v>
+      </c>
+      <c r="J87" t="b">
+        <f>TRIM(E87)=TRIM(IF(RIGHT(Sheet1!E87, 1) = ".", LEFT(Sheet1!E87, LEN(Sheet1!E87)-1),Sheet1!E87))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G88" t="b">
+        <f>TRIM(B88)=TRIM(IF(RIGHT(Sheet1!B88, 1) = ".", LEFT(Sheet1!B88, LEN(Sheet1!B88)-1),Sheet1!B88))</f>
+        <v>0</v>
+      </c>
+      <c r="H88" t="b">
+        <f>TRIM(C88)=TRIM(IF(RIGHT(Sheet1!C88, 1) = ".", LEFT(Sheet1!C88, LEN(Sheet1!C88)-1),Sheet1!C88))</f>
+        <v>0</v>
+      </c>
+      <c r="I88" t="b">
+        <f>TRIM(D88)=TRIM(IF(RIGHT(Sheet1!D88, 1) = ".", LEFT(Sheet1!D88, LEN(Sheet1!D88)-1),Sheet1!D88))</f>
+        <v>0</v>
+      </c>
+      <c r="J88" t="b">
+        <f>TRIM(E88)=TRIM(IF(RIGHT(Sheet1!E88, 1) = ".", LEFT(Sheet1!E88, LEN(Sheet1!E88)-1),Sheet1!E88))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G89" t="b">
+        <f>TRIM(B89)=TRIM(IF(RIGHT(Sheet1!B89, 1) = ".", LEFT(Sheet1!B89, LEN(Sheet1!B89)-1),Sheet1!B89))</f>
+        <v>0</v>
+      </c>
+      <c r="H89" t="b">
+        <f>TRIM(C89)=TRIM(IF(RIGHT(Sheet1!C89, 1) = ".", LEFT(Sheet1!C89, LEN(Sheet1!C89)-1),Sheet1!C89))</f>
+        <v>0</v>
+      </c>
+      <c r="I89" t="b">
+        <f>TRIM(D89)=TRIM(IF(RIGHT(Sheet1!D89, 1) = ".", LEFT(Sheet1!D89, LEN(Sheet1!D89)-1),Sheet1!D89))</f>
+        <v>0</v>
+      </c>
+      <c r="J89" t="b">
+        <f>TRIM(E89)=TRIM(IF(RIGHT(Sheet1!E89, 1) = ".", LEFT(Sheet1!E89, LEN(Sheet1!E89)-1),Sheet1!E89))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G90" t="b">
+        <f>TRIM(B90)=TRIM(IF(RIGHT(Sheet1!B90, 1) = ".", LEFT(Sheet1!B90, LEN(Sheet1!B90)-1),Sheet1!B90))</f>
+        <v>0</v>
+      </c>
+      <c r="H90" t="b">
+        <f>TRIM(C90)=TRIM(IF(RIGHT(Sheet1!C90, 1) = ".", LEFT(Sheet1!C90, LEN(Sheet1!C90)-1),Sheet1!C90))</f>
+        <v>0</v>
+      </c>
+      <c r="I90" t="b">
+        <f>TRIM(D90)=TRIM(IF(RIGHT(Sheet1!D90, 1) = ".", LEFT(Sheet1!D90, LEN(Sheet1!D90)-1),Sheet1!D90))</f>
+        <v>0</v>
+      </c>
+      <c r="J90" t="b">
+        <f>TRIM(E90)=TRIM(IF(RIGHT(Sheet1!E90, 1) = ".", LEFT(Sheet1!E90, LEN(Sheet1!E90)-1),Sheet1!E90))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G91" t="b">
+        <f>TRIM(B91)=TRIM(IF(RIGHT(Sheet1!B91, 1) = ".", LEFT(Sheet1!B91, LEN(Sheet1!B91)-1),Sheet1!B91))</f>
+        <v>0</v>
+      </c>
+      <c r="H91" t="b">
+        <f>TRIM(C91)=TRIM(IF(RIGHT(Sheet1!C91, 1) = ".", LEFT(Sheet1!C91, LEN(Sheet1!C91)-1),Sheet1!C91))</f>
+        <v>0</v>
+      </c>
+      <c r="I91" t="b">
+        <f>TRIM(D91)=TRIM(IF(RIGHT(Sheet1!D91, 1) = ".", LEFT(Sheet1!D91, LEN(Sheet1!D91)-1),Sheet1!D91))</f>
+        <v>0</v>
+      </c>
+      <c r="J91" t="b">
+        <f>TRIM(E91)=TRIM(IF(RIGHT(Sheet1!E91, 1) = ".", LEFT(Sheet1!E91, LEN(Sheet1!E91)-1),Sheet1!E91))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G92" t="b">
+        <f>TRIM(B92)=TRIM(IF(RIGHT(Sheet1!B92, 1) = ".", LEFT(Sheet1!B92, LEN(Sheet1!B92)-1),Sheet1!B92))</f>
+        <v>0</v>
+      </c>
+      <c r="H92" t="b">
+        <f>TRIM(C92)=TRIM(IF(RIGHT(Sheet1!C92, 1) = ".", LEFT(Sheet1!C92, LEN(Sheet1!C92)-1),Sheet1!C92))</f>
+        <v>0</v>
+      </c>
+      <c r="I92" t="b">
+        <f>TRIM(D92)=TRIM(IF(RIGHT(Sheet1!D92, 1) = ".", LEFT(Sheet1!D92, LEN(Sheet1!D92)-1),Sheet1!D92))</f>
+        <v>0</v>
+      </c>
+      <c r="J92" t="b">
+        <f>TRIM(E92)=TRIM(IF(RIGHT(Sheet1!E92, 1) = ".", LEFT(Sheet1!E92, LEN(Sheet1!E92)-1),Sheet1!E92))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G93" t="b">
+        <f>TRIM(B93)=TRIM(IF(RIGHT(Sheet1!B93, 1) = ".", LEFT(Sheet1!B93, LEN(Sheet1!B93)-1),Sheet1!B93))</f>
+        <v>0</v>
+      </c>
+      <c r="H93" t="b">
+        <f>TRIM(C93)=TRIM(IF(RIGHT(Sheet1!C93, 1) = ".", LEFT(Sheet1!C93, LEN(Sheet1!C93)-1),Sheet1!C93))</f>
+        <v>0</v>
+      </c>
+      <c r="I93" t="b">
+        <f>TRIM(D93)=TRIM(IF(RIGHT(Sheet1!D93, 1) = ".", LEFT(Sheet1!D93, LEN(Sheet1!D93)-1),Sheet1!D93))</f>
+        <v>0</v>
+      </c>
+      <c r="J93" t="b">
+        <f>TRIM(E93)=TRIM(IF(RIGHT(Sheet1!E93, 1) = ".", LEFT(Sheet1!E93, LEN(Sheet1!E93)-1),Sheet1!E93))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G94" t="b">
+        <f>TRIM(B94)=TRIM(IF(RIGHT(Sheet1!B94, 1) = ".", LEFT(Sheet1!B94, LEN(Sheet1!B94)-1),Sheet1!B94))</f>
+        <v>0</v>
+      </c>
+      <c r="H94" t="b">
+        <f>TRIM(C94)=TRIM(IF(RIGHT(Sheet1!C94, 1) = ".", LEFT(Sheet1!C94, LEN(Sheet1!C94)-1),Sheet1!C94))</f>
+        <v>0</v>
+      </c>
+      <c r="I94" t="b">
+        <f>TRIM(D94)=TRIM(IF(RIGHT(Sheet1!D94, 1) = ".", LEFT(Sheet1!D94, LEN(Sheet1!D94)-1),Sheet1!D94))</f>
+        <v>0</v>
+      </c>
+      <c r="J94" t="b">
+        <f>TRIM(E94)=TRIM(IF(RIGHT(Sheet1!E94, 1) = ".", LEFT(Sheet1!E94, LEN(Sheet1!E94)-1),Sheet1!E94))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G95" t="b">
+        <f>TRIM(B95)=TRIM(IF(RIGHT(Sheet1!B95, 1) = ".", LEFT(Sheet1!B95, LEN(Sheet1!B95)-1),Sheet1!B95))</f>
+        <v>0</v>
+      </c>
+      <c r="H95" t="b">
+        <f>TRIM(C95)=TRIM(IF(RIGHT(Sheet1!C95, 1) = ".", LEFT(Sheet1!C95, LEN(Sheet1!C95)-1),Sheet1!C95))</f>
+        <v>0</v>
+      </c>
+      <c r="I95" t="b">
+        <f>TRIM(D95)=TRIM(IF(RIGHT(Sheet1!D95, 1) = ".", LEFT(Sheet1!D95, LEN(Sheet1!D95)-1),Sheet1!D95))</f>
+        <v>0</v>
+      </c>
+      <c r="J95" t="b">
+        <f>TRIM(E95)=TRIM(IF(RIGHT(Sheet1!E95, 1) = ".", LEFT(Sheet1!E95, LEN(Sheet1!E95)-1),Sheet1!E95))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G96" t="b">
+        <f>TRIM(B96)=TRIM(IF(RIGHT(Sheet1!B96, 1) = ".", LEFT(Sheet1!B96, LEN(Sheet1!B96)-1),Sheet1!B96))</f>
+        <v>0</v>
+      </c>
+      <c r="H96" t="b">
+        <f>TRIM(C96)=TRIM(IF(RIGHT(Sheet1!C96, 1) = ".", LEFT(Sheet1!C96, LEN(Sheet1!C96)-1),Sheet1!C96))</f>
+        <v>0</v>
+      </c>
+      <c r="I96" t="b">
+        <f>TRIM(D96)=TRIM(IF(RIGHT(Sheet1!D96, 1) = ".", LEFT(Sheet1!D96, LEN(Sheet1!D96)-1),Sheet1!D96))</f>
+        <v>0</v>
+      </c>
+      <c r="J96" t="b">
+        <f>TRIM(E96)=TRIM(IF(RIGHT(Sheet1!E96, 1) = ".", LEFT(Sheet1!E96, LEN(Sheet1!E96)-1),Sheet1!E96))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G97" t="b">
+        <f>TRIM(B97)=TRIM(IF(RIGHT(Sheet1!B97, 1) = ".", LEFT(Sheet1!B97, LEN(Sheet1!B97)-1),Sheet1!B97))</f>
+        <v>0</v>
+      </c>
+      <c r="H97" t="b">
+        <f>TRIM(C97)=TRIM(IF(RIGHT(Sheet1!C97, 1) = ".", LEFT(Sheet1!C97, LEN(Sheet1!C97)-1),Sheet1!C97))</f>
+        <v>0</v>
+      </c>
+      <c r="I97" t="b">
+        <f>TRIM(D97)=TRIM(IF(RIGHT(Sheet1!D97, 1) = ".", LEFT(Sheet1!D97, LEN(Sheet1!D97)-1),Sheet1!D97))</f>
+        <v>0</v>
+      </c>
+      <c r="J97" t="b">
+        <f>TRIM(E97)=TRIM(IF(RIGHT(Sheet1!E97, 1) = ".", LEFT(Sheet1!E97, LEN(Sheet1!E97)-1),Sheet1!E97))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G98" t="b">
+        <f>TRIM(B98)=TRIM(IF(RIGHT(Sheet1!B98, 1) = ".", LEFT(Sheet1!B98, LEN(Sheet1!B98)-1),Sheet1!B98))</f>
+        <v>0</v>
+      </c>
+      <c r="H98" t="b">
+        <f>TRIM(C98)=TRIM(IF(RIGHT(Sheet1!C98, 1) = ".", LEFT(Sheet1!C98, LEN(Sheet1!C98)-1),Sheet1!C98))</f>
+        <v>0</v>
+      </c>
+      <c r="I98" t="b">
+        <f>TRIM(D98)=TRIM(IF(RIGHT(Sheet1!D98, 1) = ".", LEFT(Sheet1!D98, LEN(Sheet1!D98)-1),Sheet1!D98))</f>
+        <v>0</v>
+      </c>
+      <c r="J98" t="b">
+        <f>TRIM(E98)=TRIM(IF(RIGHT(Sheet1!E98, 1) = ".", LEFT(Sheet1!E98, LEN(Sheet1!E98)-1),Sheet1!E98))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G99" t="b">
+        <f>TRIM(B99)=TRIM(IF(RIGHT(Sheet1!B99, 1) = ".", LEFT(Sheet1!B99, LEN(Sheet1!B99)-1),Sheet1!B99))</f>
+        <v>0</v>
+      </c>
+      <c r="H99" t="b">
+        <f>TRIM(C99)=TRIM(IF(RIGHT(Sheet1!C99, 1) = ".", LEFT(Sheet1!C99, LEN(Sheet1!C99)-1),Sheet1!C99))</f>
+        <v>0</v>
+      </c>
+      <c r="I99" t="b">
+        <f>TRIM(D99)=TRIM(IF(RIGHT(Sheet1!D99, 1) = ".", LEFT(Sheet1!D99, LEN(Sheet1!D99)-1),Sheet1!D99))</f>
+        <v>0</v>
+      </c>
+      <c r="J99" t="b">
+        <f>TRIM(E99)=TRIM(IF(RIGHT(Sheet1!E99, 1) = ".", LEFT(Sheet1!E99, LEN(Sheet1!E99)-1),Sheet1!E99))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G100" t="b">
+        <f>TRIM(B100)=TRIM(IF(RIGHT(Sheet1!B100, 1) = ".", LEFT(Sheet1!B100, LEN(Sheet1!B100)-1),Sheet1!B100))</f>
+        <v>0</v>
+      </c>
+      <c r="H100" t="b">
+        <f>TRIM(C100)=TRIM(IF(RIGHT(Sheet1!C100, 1) = ".", LEFT(Sheet1!C100, LEN(Sheet1!C100)-1),Sheet1!C100))</f>
+        <v>0</v>
+      </c>
+      <c r="I100" t="b">
+        <f>TRIM(D100)=TRIM(IF(RIGHT(Sheet1!D100, 1) = ".", LEFT(Sheet1!D100, LEN(Sheet1!D100)-1),Sheet1!D100))</f>
+        <v>0</v>
+      </c>
+      <c r="J100" t="b">
+        <f>TRIM(E100)=TRIM(IF(RIGHT(Sheet1!E100, 1) = ".", LEFT(Sheet1!E100, LEN(Sheet1!E100)-1),Sheet1!E100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G101" t="b">
+        <f>TRIM(B101)=TRIM(IF(RIGHT(Sheet1!B101, 1) = ".", LEFT(Sheet1!B101, LEN(Sheet1!B101)-1),Sheet1!B101))</f>
+        <v>0</v>
+      </c>
+      <c r="H101" t="b">
+        <f>TRIM(C101)=TRIM(IF(RIGHT(Sheet1!C101, 1) = ".", LEFT(Sheet1!C101, LEN(Sheet1!C101)-1),Sheet1!C101))</f>
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <f>TRIM(D101)=TRIM(IF(RIGHT(Sheet1!D101, 1) = ".", LEFT(Sheet1!D101, LEN(Sheet1!D101)-1),Sheet1!D101))</f>
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <f>TRIM(E101)=TRIM(IF(RIGHT(Sheet1!E101, 1) = ".", LEFT(Sheet1!E101, LEN(Sheet1!E101)-1),Sheet1!E101))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G102" t="b">
+        <f>TRIM(B102)=TRIM(IF(RIGHT(Sheet1!B102, 1) = ".", LEFT(Sheet1!B102, LEN(Sheet1!B102)-1),Sheet1!B102))</f>
+        <v>0</v>
+      </c>
+      <c r="H102" t="b">
+        <f>TRIM(C102)=TRIM(IF(RIGHT(Sheet1!C102, 1) = ".", LEFT(Sheet1!C102, LEN(Sheet1!C102)-1),Sheet1!C102))</f>
+        <v>0</v>
+      </c>
+      <c r="I102" t="b">
+        <f>TRIM(D102)=TRIM(IF(RIGHT(Sheet1!D102, 1) = ".", LEFT(Sheet1!D102, LEN(Sheet1!D102)-1),Sheet1!D102))</f>
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <f>TRIM(E102)=TRIM(IF(RIGHT(Sheet1!E102, 1) = ".", LEFT(Sheet1!E102, LEN(Sheet1!E102)-1),Sheet1!E102))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G103" t="b">
+        <f>TRIM(B103)=TRIM(IF(RIGHT(Sheet1!B103, 1) = ".", LEFT(Sheet1!B103, LEN(Sheet1!B103)-1),Sheet1!B103))</f>
+        <v>0</v>
+      </c>
+      <c r="H103" t="b">
+        <f>TRIM(C103)=TRIM(IF(RIGHT(Sheet1!C103, 1) = ".", LEFT(Sheet1!C103, LEN(Sheet1!C103)-1),Sheet1!C103))</f>
+        <v>0</v>
+      </c>
+      <c r="I103" t="b">
+        <f>TRIM(D103)=TRIM(IF(RIGHT(Sheet1!D103, 1) = ".", LEFT(Sheet1!D103, LEN(Sheet1!D103)-1),Sheet1!D103))</f>
+        <v>0</v>
+      </c>
+      <c r="J103" t="b">
+        <f>TRIM(E103)=TRIM(IF(RIGHT(Sheet1!E103, 1) = ".", LEFT(Sheet1!E103, LEN(Sheet1!E103)-1),Sheet1!E103))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G104" t="b">
+        <f>TRIM(B104)=TRIM(IF(RIGHT(Sheet1!B104, 1) = ".", LEFT(Sheet1!B104, LEN(Sheet1!B104)-1),Sheet1!B104))</f>
+        <v>0</v>
+      </c>
+      <c r="H104" t="b">
+        <f>TRIM(C104)=TRIM(IF(RIGHT(Sheet1!C104, 1) = ".", LEFT(Sheet1!C104, LEN(Sheet1!C104)-1),Sheet1!C104))</f>
+        <v>0</v>
+      </c>
+      <c r="I104" t="b">
+        <f>TRIM(D104)=TRIM(IF(RIGHT(Sheet1!D104, 1) = ".", LEFT(Sheet1!D104, LEN(Sheet1!D104)-1),Sheet1!D104))</f>
+        <v>0</v>
+      </c>
+      <c r="J104" t="b">
+        <f>TRIM(E104)=TRIM(IF(RIGHT(Sheet1!E104, 1) = ".", LEFT(Sheet1!E104, LEN(Sheet1!E104)-1),Sheet1!E104))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G105" t="b">
+        <f>TRIM(B105)=TRIM(IF(RIGHT(Sheet1!B105, 1) = ".", LEFT(Sheet1!B105, LEN(Sheet1!B105)-1),Sheet1!B105))</f>
+        <v>0</v>
+      </c>
+      <c r="H105" t="b">
+        <f>TRIM(C105)=TRIM(IF(RIGHT(Sheet1!C105, 1) = ".", LEFT(Sheet1!C105, LEN(Sheet1!C105)-1),Sheet1!C105))</f>
+        <v>0</v>
+      </c>
+      <c r="I105" t="b">
+        <f>TRIM(D105)=TRIM(IF(RIGHT(Sheet1!D105, 1) = ".", LEFT(Sheet1!D105, LEN(Sheet1!D105)-1),Sheet1!D105))</f>
+        <v>0</v>
+      </c>
+      <c r="J105" t="b">
+        <f>TRIM(E105)=TRIM(IF(RIGHT(Sheet1!E105, 1) = ".", LEFT(Sheet1!E105, LEN(Sheet1!E105)-1),Sheet1!E105))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G106" t="b">
+        <f>TRIM(B106)=TRIM(IF(RIGHT(Sheet1!B106, 1) = ".", LEFT(Sheet1!B106, LEN(Sheet1!B106)-1),Sheet1!B106))</f>
+        <v>0</v>
+      </c>
+      <c r="H106" t="b">
+        <f>TRIM(C106)=TRIM(IF(RIGHT(Sheet1!C106, 1) = ".", LEFT(Sheet1!C106, LEN(Sheet1!C106)-1),Sheet1!C106))</f>
+        <v>0</v>
+      </c>
+      <c r="I106" t="b">
+        <f>TRIM(D106)=TRIM(IF(RIGHT(Sheet1!D106, 1) = ".", LEFT(Sheet1!D106, LEN(Sheet1!D106)-1),Sheet1!D106))</f>
+        <v>0</v>
+      </c>
+      <c r="J106" t="b">
+        <f>TRIM(E106)=TRIM(IF(RIGHT(Sheet1!E106, 1) = ".", LEFT(Sheet1!E106, LEN(Sheet1!E106)-1),Sheet1!E106))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G107" t="b">
+        <f>TRIM(B107)=TRIM(IF(RIGHT(Sheet1!B107, 1) = ".", LEFT(Sheet1!B107, LEN(Sheet1!B107)-1),Sheet1!B107))</f>
+        <v>0</v>
+      </c>
+      <c r="H107" t="b">
+        <f>TRIM(C107)=TRIM(IF(RIGHT(Sheet1!C107, 1) = ".", LEFT(Sheet1!C107, LEN(Sheet1!C107)-1),Sheet1!C107))</f>
+        <v>0</v>
+      </c>
+      <c r="I107" t="b">
+        <f>TRIM(D107)=TRIM(IF(RIGHT(Sheet1!D107, 1) = ".", LEFT(Sheet1!D107, LEN(Sheet1!D107)-1),Sheet1!D107))</f>
+        <v>0</v>
+      </c>
+      <c r="J107" t="b">
+        <f>TRIM(E107)=TRIM(IF(RIGHT(Sheet1!E107, 1) = ".", LEFT(Sheet1!E107, LEN(Sheet1!E107)-1),Sheet1!E107))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G108" t="b">
+        <f>TRIM(B108)=TRIM(IF(RIGHT(Sheet1!B108, 1) = ".", LEFT(Sheet1!B108, LEN(Sheet1!B108)-1),Sheet1!B108))</f>
+        <v>0</v>
+      </c>
+      <c r="H108" t="b">
+        <f>TRIM(C108)=TRIM(IF(RIGHT(Sheet1!C108, 1) = ".", LEFT(Sheet1!C108, LEN(Sheet1!C108)-1),Sheet1!C108))</f>
+        <v>0</v>
+      </c>
+      <c r="I108" t="b">
+        <f>TRIM(D108)=TRIM(IF(RIGHT(Sheet1!D108, 1) = ".", LEFT(Sheet1!D108, LEN(Sheet1!D108)-1),Sheet1!D108))</f>
+        <v>0</v>
+      </c>
+      <c r="J108" t="b">
+        <f>TRIM(E108)=TRIM(IF(RIGHT(Sheet1!E108, 1) = ".", LEFT(Sheet1!E108, LEN(Sheet1!E108)-1),Sheet1!E108))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G109" t="b">
+        <f>TRIM(B109)=TRIM(IF(RIGHT(Sheet1!B109, 1) = ".", LEFT(Sheet1!B109, LEN(Sheet1!B109)-1),Sheet1!B109))</f>
+        <v>0</v>
+      </c>
+      <c r="H109" t="b">
+        <f>TRIM(C109)=TRIM(IF(RIGHT(Sheet1!C109, 1) = ".", LEFT(Sheet1!C109, LEN(Sheet1!C109)-1),Sheet1!C109))</f>
+        <v>0</v>
+      </c>
+      <c r="I109" t="b">
+        <f>TRIM(D109)=TRIM(IF(RIGHT(Sheet1!D109, 1) = ".", LEFT(Sheet1!D109, LEN(Sheet1!D109)-1),Sheet1!D109))</f>
+        <v>0</v>
+      </c>
+      <c r="J109" t="b">
+        <f>TRIM(E109)=TRIM(IF(RIGHT(Sheet1!E109, 1) = ".", LEFT(Sheet1!E109, LEN(Sheet1!E109)-1),Sheet1!E109))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G110" t="b">
+        <f>TRIM(B110)=TRIM(IF(RIGHT(Sheet1!B110, 1) = ".", LEFT(Sheet1!B110, LEN(Sheet1!B110)-1),Sheet1!B110))</f>
+        <v>0</v>
+      </c>
+      <c r="H110" t="b">
+        <f>TRIM(C110)=TRIM(IF(RIGHT(Sheet1!C110, 1) = ".", LEFT(Sheet1!C110, LEN(Sheet1!C110)-1),Sheet1!C110))</f>
+        <v>0</v>
+      </c>
+      <c r="I110" t="b">
+        <f>TRIM(D110)=TRIM(IF(RIGHT(Sheet1!D110, 1) = ".", LEFT(Sheet1!D110, LEN(Sheet1!D110)-1),Sheet1!D110))</f>
+        <v>0</v>
+      </c>
+      <c r="J110" t="b">
+        <f>TRIM(E110)=TRIM(IF(RIGHT(Sheet1!E110, 1) = ".", LEFT(Sheet1!E110, LEN(Sheet1!E110)-1),Sheet1!E110))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G111" t="b">
+        <f>TRIM(B111)=TRIM(IF(RIGHT(Sheet1!B111, 1) = ".", LEFT(Sheet1!B111, LEN(Sheet1!B111)-1),Sheet1!B111))</f>
+        <v>0</v>
+      </c>
+      <c r="H111" t="b">
+        <f>TRIM(C111)=TRIM(IF(RIGHT(Sheet1!C111, 1) = ".", LEFT(Sheet1!C111, LEN(Sheet1!C111)-1),Sheet1!C111))</f>
+        <v>0</v>
+      </c>
+      <c r="I111" t="b">
+        <f>TRIM(D111)=TRIM(IF(RIGHT(Sheet1!D111, 1) = ".", LEFT(Sheet1!D111, LEN(Sheet1!D111)-1),Sheet1!D111))</f>
+        <v>0</v>
+      </c>
+      <c r="J111" t="b">
+        <f>TRIM(E111)=TRIM(IF(RIGHT(Sheet1!E111, 1) = ".", LEFT(Sheet1!E111, LEN(Sheet1!E111)-1),Sheet1!E111))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G112" t="b">
+        <f>TRIM(B112)=TRIM(IF(RIGHT(Sheet1!B112, 1) = ".", LEFT(Sheet1!B112, LEN(Sheet1!B112)-1),Sheet1!B112))</f>
+        <v>0</v>
+      </c>
+      <c r="H112" t="b">
+        <f>TRIM(C112)=TRIM(IF(RIGHT(Sheet1!C112, 1) = ".", LEFT(Sheet1!C112, LEN(Sheet1!C112)-1),Sheet1!C112))</f>
+        <v>0</v>
+      </c>
+      <c r="I112" t="b">
+        <f>TRIM(D112)=TRIM(IF(RIGHT(Sheet1!D112, 1) = ".", LEFT(Sheet1!D112, LEN(Sheet1!D112)-1),Sheet1!D112))</f>
+        <v>0</v>
+      </c>
+      <c r="J112" t="b">
+        <f>TRIM(E112)=TRIM(IF(RIGHT(Sheet1!E112, 1) = ".", LEFT(Sheet1!E112, LEN(Sheet1!E112)-1),Sheet1!E112))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G113" t="b">
+        <f>TRIM(B113)=TRIM(IF(RIGHT(Sheet1!B113, 1) = ".", LEFT(Sheet1!B113, LEN(Sheet1!B113)-1),Sheet1!B113))</f>
+        <v>0</v>
+      </c>
+      <c r="H113" t="b">
+        <f>TRIM(C113)=TRIM(IF(RIGHT(Sheet1!C113, 1) = ".", LEFT(Sheet1!C113, LEN(Sheet1!C113)-1),Sheet1!C113))</f>
+        <v>0</v>
+      </c>
+      <c r="I113" t="b">
+        <f>TRIM(D113)=TRIM(IF(RIGHT(Sheet1!D113, 1) = ".", LEFT(Sheet1!D113, LEN(Sheet1!D113)-1),Sheet1!D113))</f>
+        <v>0</v>
+      </c>
+      <c r="J113" t="b">
+        <f>TRIM(E113)=TRIM(IF(RIGHT(Sheet1!E113, 1) = ".", LEFT(Sheet1!E113, LEN(Sheet1!E113)-1),Sheet1!E113))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G114" t="b">
+        <f>TRIM(B114)=TRIM(IF(RIGHT(Sheet1!B114, 1) = ".", LEFT(Sheet1!B114, LEN(Sheet1!B114)-1),Sheet1!B114))</f>
+        <v>0</v>
+      </c>
+      <c r="H114" t="b">
+        <f>TRIM(C114)=TRIM(IF(RIGHT(Sheet1!C114, 1) = ".", LEFT(Sheet1!C114, LEN(Sheet1!C114)-1),Sheet1!C114))</f>
+        <v>0</v>
+      </c>
+      <c r="I114" t="b">
+        <f>TRIM(D114)=TRIM(IF(RIGHT(Sheet1!D114, 1) = ".", LEFT(Sheet1!D114, LEN(Sheet1!D114)-1),Sheet1!D114))</f>
+        <v>0</v>
+      </c>
+      <c r="J114" t="b">
+        <f>TRIM(E114)=TRIM(IF(RIGHT(Sheet1!E114, 1) = ".", LEFT(Sheet1!E114, LEN(Sheet1!E114)-1),Sheet1!E114))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G115" t="b">
+        <f>TRIM(B115)=TRIM(IF(RIGHT(Sheet1!B115, 1) = ".", LEFT(Sheet1!B115, LEN(Sheet1!B115)-1),Sheet1!B115))</f>
+        <v>0</v>
+      </c>
+      <c r="H115" t="b">
+        <f>TRIM(C115)=TRIM(IF(RIGHT(Sheet1!C115, 1) = ".", LEFT(Sheet1!C115, LEN(Sheet1!C115)-1),Sheet1!C115))</f>
+        <v>0</v>
+      </c>
+      <c r="I115" t="b">
+        <f>TRIM(D115)=TRIM(IF(RIGHT(Sheet1!D115, 1) = ".", LEFT(Sheet1!D115, LEN(Sheet1!D115)-1),Sheet1!D115))</f>
+        <v>0</v>
+      </c>
+      <c r="J115" t="b">
+        <f>TRIM(E115)=TRIM(IF(RIGHT(Sheet1!E115, 1) = ".", LEFT(Sheet1!E115, LEN(Sheet1!E115)-1),Sheet1!E115))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G116" t="b">
+        <f>TRIM(B116)=TRIM(IF(RIGHT(Sheet1!B116, 1) = ".", LEFT(Sheet1!B116, LEN(Sheet1!B116)-1),Sheet1!B116))</f>
+        <v>0</v>
+      </c>
+      <c r="H116" t="b">
+        <f>TRIM(C116)=TRIM(IF(RIGHT(Sheet1!C116, 1) = ".", LEFT(Sheet1!C116, LEN(Sheet1!C116)-1),Sheet1!C116))</f>
+        <v>0</v>
+      </c>
+      <c r="I116" t="b">
+        <f>TRIM(D116)=TRIM(IF(RIGHT(Sheet1!D116, 1) = ".", LEFT(Sheet1!D116, LEN(Sheet1!D116)-1),Sheet1!D116))</f>
+        <v>0</v>
+      </c>
+      <c r="J116" t="b">
+        <f>TRIM(E116)=TRIM(IF(RIGHT(Sheet1!E116, 1) = ".", LEFT(Sheet1!E116, LEN(Sheet1!E116)-1),Sheet1!E116))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G117" t="b">
+        <f>TRIM(B117)=TRIM(IF(RIGHT(Sheet1!B117, 1) = ".", LEFT(Sheet1!B117, LEN(Sheet1!B117)-1),Sheet1!B117))</f>
+        <v>0</v>
+      </c>
+      <c r="H117" t="b">
+        <f>TRIM(C117)=TRIM(IF(RIGHT(Sheet1!C117, 1) = ".", LEFT(Sheet1!C117, LEN(Sheet1!C117)-1),Sheet1!C117))</f>
+        <v>0</v>
+      </c>
+      <c r="I117" t="b">
+        <f>TRIM(D117)=TRIM(IF(RIGHT(Sheet1!D117, 1) = ".", LEFT(Sheet1!D117, LEN(Sheet1!D117)-1),Sheet1!D117))</f>
+        <v>0</v>
+      </c>
+      <c r="J117" t="b">
+        <f>TRIM(E117)=TRIM(IF(RIGHT(Sheet1!E117, 1) = ".", LEFT(Sheet1!E117, LEN(Sheet1!E117)-1),Sheet1!E117))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G118" t="b">
+        <f>TRIM(B118)=TRIM(IF(RIGHT(Sheet1!B118, 1) = ".", LEFT(Sheet1!B118, LEN(Sheet1!B118)-1),Sheet1!B118))</f>
+        <v>0</v>
+      </c>
+      <c r="H118" t="b">
+        <f>TRIM(C118)=TRIM(IF(RIGHT(Sheet1!C118, 1) = ".", LEFT(Sheet1!C118, LEN(Sheet1!C118)-1),Sheet1!C118))</f>
+        <v>0</v>
+      </c>
+      <c r="I118" t="b">
+        <f>TRIM(D118)=TRIM(IF(RIGHT(Sheet1!D118, 1) = ".", LEFT(Sheet1!D118, LEN(Sheet1!D118)-1),Sheet1!D118))</f>
+        <v>0</v>
+      </c>
+      <c r="J118" t="b">
+        <f>TRIM(E118)=TRIM(IF(RIGHT(Sheet1!E118, 1) = ".", LEFT(Sheet1!E118, LEN(Sheet1!E118)-1),Sheet1!E118))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G119" t="b">
+        <f>TRIM(B119)=TRIM(IF(RIGHT(Sheet1!B119, 1) = ".", LEFT(Sheet1!B119, LEN(Sheet1!B119)-1),Sheet1!B119))</f>
+        <v>0</v>
+      </c>
+      <c r="H119" t="b">
+        <f>TRIM(C119)=TRIM(IF(RIGHT(Sheet1!C119, 1) = ".", LEFT(Sheet1!C119, LEN(Sheet1!C119)-1),Sheet1!C119))</f>
+        <v>0</v>
+      </c>
+      <c r="I119" t="b">
+        <f>TRIM(D119)=TRIM(IF(RIGHT(Sheet1!D119, 1) = ".", LEFT(Sheet1!D119, LEN(Sheet1!D119)-1),Sheet1!D119))</f>
+        <v>0</v>
+      </c>
+      <c r="J119" t="b">
+        <f>TRIM(E119)=TRIM(IF(RIGHT(Sheet1!E119, 1) = ".", LEFT(Sheet1!E119, LEN(Sheet1!E119)-1),Sheet1!E119))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G120" t="b">
+        <f>TRIM(B120)=TRIM(IF(RIGHT(Sheet1!B120, 1) = ".", LEFT(Sheet1!B120, LEN(Sheet1!B120)-1),Sheet1!B120))</f>
+        <v>0</v>
+      </c>
+      <c r="H120" t="b">
+        <f>TRIM(C120)=TRIM(IF(RIGHT(Sheet1!C120, 1) = ".", LEFT(Sheet1!C120, LEN(Sheet1!C120)-1),Sheet1!C120))</f>
+        <v>0</v>
+      </c>
+      <c r="I120" t="b">
+        <f>TRIM(D120)=TRIM(IF(RIGHT(Sheet1!D120, 1) = ".", LEFT(Sheet1!D120, LEN(Sheet1!D120)-1),Sheet1!D120))</f>
+        <v>0</v>
+      </c>
+      <c r="J120" t="b">
+        <f>TRIM(E120)=TRIM(IF(RIGHT(Sheet1!E120, 1) = ".", LEFT(Sheet1!E120, LEN(Sheet1!E120)-1),Sheet1!E120))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G121" t="b">
+        <f>TRIM(B121)=TRIM(IF(RIGHT(Sheet1!B121, 1) = ".", LEFT(Sheet1!B121, LEN(Sheet1!B121)-1),Sheet1!B121))</f>
+        <v>0</v>
+      </c>
+      <c r="H121" t="b">
+        <f>TRIM(C121)=TRIM(IF(RIGHT(Sheet1!C121, 1) = ".", LEFT(Sheet1!C121, LEN(Sheet1!C121)-1),Sheet1!C121))</f>
+        <v>0</v>
+      </c>
+      <c r="I121" t="b">
+        <f>TRIM(D121)=TRIM(IF(RIGHT(Sheet1!D121, 1) = ".", LEFT(Sheet1!D121, LEN(Sheet1!D121)-1),Sheet1!D121))</f>
+        <v>0</v>
+      </c>
+      <c r="J121" t="b">
+        <f>TRIM(E121)=TRIM(IF(RIGHT(Sheet1!E121, 1) = ".", LEFT(Sheet1!E121, LEN(Sheet1!E121)-1),Sheet1!E121))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G122" t="b">
+        <f>TRIM(B122)=TRIM(IF(RIGHT(Sheet1!B122, 1) = ".", LEFT(Sheet1!B122, LEN(Sheet1!B122)-1),Sheet1!B122))</f>
+        <v>0</v>
+      </c>
+      <c r="H122" t="b">
+        <f>TRIM(C122)=TRIM(IF(RIGHT(Sheet1!C122, 1) = ".", LEFT(Sheet1!C122, LEN(Sheet1!C122)-1),Sheet1!C122))</f>
+        <v>0</v>
+      </c>
+      <c r="I122" t="b">
+        <f>TRIM(D122)=TRIM(IF(RIGHT(Sheet1!D122, 1) = ".", LEFT(Sheet1!D122, LEN(Sheet1!D122)-1),Sheet1!D122))</f>
+        <v>0</v>
+      </c>
+      <c r="J122" t="b">
+        <f>TRIM(E122)=TRIM(IF(RIGHT(Sheet1!E122, 1) = ".", LEFT(Sheet1!E122, LEN(Sheet1!E122)-1),Sheet1!E122))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G123" t="b">
+        <f>TRIM(B123)=TRIM(IF(RIGHT(Sheet1!B123, 1) = ".", LEFT(Sheet1!B123, LEN(Sheet1!B123)-1),Sheet1!B123))</f>
+        <v>0</v>
+      </c>
+      <c r="H123" t="b">
+        <f>TRIM(C123)=TRIM(IF(RIGHT(Sheet1!C123, 1) = ".", LEFT(Sheet1!C123, LEN(Sheet1!C123)-1),Sheet1!C123))</f>
+        <v>0</v>
+      </c>
+      <c r="I123" t="b">
+        <f>TRIM(D123)=TRIM(IF(RIGHT(Sheet1!D123, 1) = ".", LEFT(Sheet1!D123, LEN(Sheet1!D123)-1),Sheet1!D123))</f>
+        <v>0</v>
+      </c>
+      <c r="J123" t="b">
+        <f>TRIM(E123)=TRIM(IF(RIGHT(Sheet1!E123, 1) = ".", LEFT(Sheet1!E123, LEN(Sheet1!E123)-1),Sheet1!E123))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G124" t="b">
+        <f>TRIM(B124)=TRIM(IF(RIGHT(Sheet1!B124, 1) = ".", LEFT(Sheet1!B124, LEN(Sheet1!B124)-1),Sheet1!B124))</f>
+        <v>0</v>
+      </c>
+      <c r="H124" t="b">
+        <f>TRIM(C124)=TRIM(IF(RIGHT(Sheet1!C124, 1) = ".", LEFT(Sheet1!C124, LEN(Sheet1!C124)-1),Sheet1!C124))</f>
+        <v>0</v>
+      </c>
+      <c r="I124" t="b">
+        <f>TRIM(D124)=TRIM(IF(RIGHT(Sheet1!D124, 1) = ".", LEFT(Sheet1!D124, LEN(Sheet1!D124)-1),Sheet1!D124))</f>
+        <v>0</v>
+      </c>
+      <c r="J124" t="b">
+        <f>TRIM(E124)=TRIM(IF(RIGHT(Sheet1!E124, 1) = ".", LEFT(Sheet1!E124, LEN(Sheet1!E124)-1),Sheet1!E124))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G125" t="b">
+        <f>TRIM(B125)=TRIM(IF(RIGHT(Sheet1!B125, 1) = ".", LEFT(Sheet1!B125, LEN(Sheet1!B125)-1),Sheet1!B125))</f>
+        <v>0</v>
+      </c>
+      <c r="H125" t="b">
+        <f>TRIM(C125)=TRIM(IF(RIGHT(Sheet1!C125, 1) = ".", LEFT(Sheet1!C125, LEN(Sheet1!C125)-1),Sheet1!C125))</f>
+        <v>0</v>
+      </c>
+      <c r="I125" t="b">
+        <f>TRIM(D125)=TRIM(IF(RIGHT(Sheet1!D125, 1) = ".", LEFT(Sheet1!D125, LEN(Sheet1!D125)-1),Sheet1!D125))</f>
+        <v>0</v>
+      </c>
+      <c r="J125" t="b">
+        <f>TRIM(E125)=TRIM(IF(RIGHT(Sheet1!E125, 1) = ".", LEFT(Sheet1!E125, LEN(Sheet1!E125)-1),Sheet1!E125))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G126" t="b">
+        <f>TRIM(B126)=TRIM(IF(RIGHT(Sheet1!B126, 1) = ".", LEFT(Sheet1!B126, LEN(Sheet1!B126)-1),Sheet1!B126))</f>
+        <v>0</v>
+      </c>
+      <c r="H126" t="b">
+        <f>TRIM(C126)=TRIM(IF(RIGHT(Sheet1!C126, 1) = ".", LEFT(Sheet1!C126, LEN(Sheet1!C126)-1),Sheet1!C126))</f>
+        <v>0</v>
+      </c>
+      <c r="I126" t="b">
+        <f>TRIM(D126)=TRIM(IF(RIGHT(Sheet1!D126, 1) = ".", LEFT(Sheet1!D126, LEN(Sheet1!D126)-1),Sheet1!D126))</f>
+        <v>0</v>
+      </c>
+      <c r="J126" t="b">
+        <f>TRIM(E126)=TRIM(IF(RIGHT(Sheet1!E126, 1) = ".", LEFT(Sheet1!E126, LEN(Sheet1!E126)-1),Sheet1!E126))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G127" t="b">
+        <f>TRIM(B127)=TRIM(IF(RIGHT(Sheet1!B127, 1) = ".", LEFT(Sheet1!B127, LEN(Sheet1!B127)-1),Sheet1!B127))</f>
+        <v>0</v>
+      </c>
+      <c r="H127" t="b">
+        <f>TRIM(C127)=TRIM(IF(RIGHT(Sheet1!C127, 1) = ".", LEFT(Sheet1!C127, LEN(Sheet1!C127)-1),Sheet1!C127))</f>
+        <v>0</v>
+      </c>
+      <c r="I127" t="b">
+        <f>TRIM(D127)=TRIM(IF(RIGHT(Sheet1!D127, 1) = ".", LEFT(Sheet1!D127, LEN(Sheet1!D127)-1),Sheet1!D127))</f>
+        <v>0</v>
+      </c>
+      <c r="J127" t="b">
+        <f>TRIM(E127)=TRIM(IF(RIGHT(Sheet1!E127, 1) = ".", LEFT(Sheet1!E127, LEN(Sheet1!E127)-1),Sheet1!E127))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G128" t="b">
+        <f>TRIM(B128)=TRIM(IF(RIGHT(Sheet1!B128, 1) = ".", LEFT(Sheet1!B128, LEN(Sheet1!B128)-1),Sheet1!B128))</f>
+        <v>0</v>
+      </c>
+      <c r="H128" t="b">
+        <f>TRIM(C128)=TRIM(IF(RIGHT(Sheet1!C128, 1) = ".", LEFT(Sheet1!C128, LEN(Sheet1!C128)-1),Sheet1!C128))</f>
+        <v>0</v>
+      </c>
+      <c r="I128" t="b">
+        <f>TRIM(D128)=TRIM(IF(RIGHT(Sheet1!D128, 1) = ".", LEFT(Sheet1!D128, LEN(Sheet1!D128)-1),Sheet1!D128))</f>
+        <v>0</v>
+      </c>
+      <c r="J128" t="b">
+        <f>TRIM(E128)=TRIM(IF(RIGHT(Sheet1!E128, 1) = ".", LEFT(Sheet1!E128, LEN(Sheet1!E128)-1),Sheet1!E128))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G129" t="b">
+        <f>TRIM(B129)=TRIM(IF(RIGHT(Sheet1!B129, 1) = ".", LEFT(Sheet1!B129, LEN(Sheet1!B129)-1),Sheet1!B129))</f>
+        <v>0</v>
+      </c>
+      <c r="H129" t="b">
+        <f>TRIM(C129)=TRIM(IF(RIGHT(Sheet1!C129, 1) = ".", LEFT(Sheet1!C129, LEN(Sheet1!C129)-1),Sheet1!C129))</f>
+        <v>0</v>
+      </c>
+      <c r="I129" t="b">
+        <f>TRIM(D129)=TRIM(IF(RIGHT(Sheet1!D129, 1) = ".", LEFT(Sheet1!D129, LEN(Sheet1!D129)-1),Sheet1!D129))</f>
+        <v>0</v>
+      </c>
+      <c r="J129" t="b">
+        <f>TRIM(E129)=TRIM(IF(RIGHT(Sheet1!E129, 1) = ".", LEFT(Sheet1!E129, LEN(Sheet1!E129)-1),Sheet1!E129))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G130" t="b">
+        <f>TRIM(B130)=TRIM(IF(RIGHT(Sheet1!B130, 1) = ".", LEFT(Sheet1!B130, LEN(Sheet1!B130)-1),Sheet1!B130))</f>
+        <v>0</v>
+      </c>
+      <c r="H130" t="b">
+        <f>TRIM(C130)=TRIM(IF(RIGHT(Sheet1!C130, 1) = ".", LEFT(Sheet1!C130, LEN(Sheet1!C130)-1),Sheet1!C130))</f>
+        <v>0</v>
+      </c>
+      <c r="I130" t="b">
+        <f>TRIM(D130)=TRIM(IF(RIGHT(Sheet1!D130, 1) = ".", LEFT(Sheet1!D130, LEN(Sheet1!D130)-1),Sheet1!D130))</f>
+        <v>0</v>
+      </c>
+      <c r="J130" t="b">
+        <f>TRIM(E130)=TRIM(IF(RIGHT(Sheet1!E130, 1) = ".", LEFT(Sheet1!E130, LEN(Sheet1!E130)-1),Sheet1!E130))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G131" t="b">
+        <f>TRIM(B131)=TRIM(IF(RIGHT(Sheet1!B131, 1) = ".", LEFT(Sheet1!B131, LEN(Sheet1!B131)-1),Sheet1!B131))</f>
+        <v>0</v>
+      </c>
+      <c r="H131" t="b">
+        <f>TRIM(C131)=TRIM(IF(RIGHT(Sheet1!C131, 1) = ".", LEFT(Sheet1!C131, LEN(Sheet1!C131)-1),Sheet1!C131))</f>
+        <v>0</v>
+      </c>
+      <c r="I131" t="b">
+        <f>TRIM(D131)=TRIM(IF(RIGHT(Sheet1!D131, 1) = ".", LEFT(Sheet1!D131, LEN(Sheet1!D131)-1),Sheet1!D131))</f>
+        <v>0</v>
+      </c>
+      <c r="J131" t="b">
+        <f>TRIM(E131)=TRIM(IF(RIGHT(Sheet1!E131, 1) = ".", LEFT(Sheet1!E131, LEN(Sheet1!E131)-1),Sheet1!E131))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G132" t="b">
+        <f>TRIM(B132)=TRIM(IF(RIGHT(Sheet1!B132, 1) = ".", LEFT(Sheet1!B132, LEN(Sheet1!B132)-1),Sheet1!B132))</f>
+        <v>0</v>
+      </c>
+      <c r="H132" t="b">
+        <f>TRIM(C132)=TRIM(IF(RIGHT(Sheet1!C132, 1) = ".", LEFT(Sheet1!C132, LEN(Sheet1!C132)-1),Sheet1!C132))</f>
+        <v>0</v>
+      </c>
+      <c r="I132" t="b">
+        <f>TRIM(D132)=TRIM(IF(RIGHT(Sheet1!D132, 1) = ".", LEFT(Sheet1!D132, LEN(Sheet1!D132)-1),Sheet1!D132))</f>
+        <v>0</v>
+      </c>
+      <c r="J132" t="b">
+        <f>TRIM(E132)=TRIM(IF(RIGHT(Sheet1!E132, 1) = ".", LEFT(Sheet1!E132, LEN(Sheet1!E132)-1),Sheet1!E132))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G133" t="b">
+        <f>TRIM(B133)=TRIM(IF(RIGHT(Sheet1!B133, 1) = ".", LEFT(Sheet1!B133, LEN(Sheet1!B133)-1),Sheet1!B133))</f>
+        <v>0</v>
+      </c>
+      <c r="H133" t="b">
+        <f>TRIM(C133)=TRIM(IF(RIGHT(Sheet1!C133, 1) = ".", LEFT(Sheet1!C133, LEN(Sheet1!C133)-1),Sheet1!C133))</f>
+        <v>0</v>
+      </c>
+      <c r="I133" t="b">
+        <f>TRIM(D133)=TRIM(IF(RIGHT(Sheet1!D133, 1) = ".", LEFT(Sheet1!D133, LEN(Sheet1!D133)-1),Sheet1!D133))</f>
+        <v>0</v>
+      </c>
+      <c r="J133" t="b">
+        <f>TRIM(E133)=TRIM(IF(RIGHT(Sheet1!E133, 1) = ".", LEFT(Sheet1!E133, LEN(Sheet1!E133)-1),Sheet1!E133))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G134" t="b">
+        <f>TRIM(B134)=TRIM(IF(RIGHT(Sheet1!B134, 1) = ".", LEFT(Sheet1!B134, LEN(Sheet1!B134)-1),Sheet1!B134))</f>
+        <v>0</v>
+      </c>
+      <c r="H134" t="b">
+        <f>TRIM(C134)=TRIM(IF(RIGHT(Sheet1!C134, 1) = ".", LEFT(Sheet1!C134, LEN(Sheet1!C134)-1),Sheet1!C134))</f>
+        <v>0</v>
+      </c>
+      <c r="I134" t="b">
+        <f>TRIM(D134)=TRIM(IF(RIGHT(Sheet1!D134, 1) = ".", LEFT(Sheet1!D134, LEN(Sheet1!D134)-1),Sheet1!D134))</f>
+        <v>0</v>
+      </c>
+      <c r="J134" t="b">
+        <f>TRIM(E134)=TRIM(IF(RIGHT(Sheet1!E134, 1) = ".", LEFT(Sheet1!E134, LEN(Sheet1!E134)-1),Sheet1!E134))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G135" t="b">
+        <f>TRIM(B135)=TRIM(IF(RIGHT(Sheet1!B135, 1) = ".", LEFT(Sheet1!B135, LEN(Sheet1!B135)-1),Sheet1!B135))</f>
+        <v>0</v>
+      </c>
+      <c r="H135" t="b">
+        <f>TRIM(C135)=TRIM(IF(RIGHT(Sheet1!C135, 1) = ".", LEFT(Sheet1!C135, LEN(Sheet1!C135)-1),Sheet1!C135))</f>
+        <v>0</v>
+      </c>
+      <c r="I135" t="b">
+        <f>TRIM(D135)=TRIM(IF(RIGHT(Sheet1!D135, 1) = ".", LEFT(Sheet1!D135, LEN(Sheet1!D135)-1),Sheet1!D135))</f>
+        <v>0</v>
+      </c>
+      <c r="J135" t="b">
+        <f>TRIM(E135)=TRIM(IF(RIGHT(Sheet1!E135, 1) = ".", LEFT(Sheet1!E135, LEN(Sheet1!E135)-1),Sheet1!E135))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G136" t="b">
+        <f>TRIM(B136)=TRIM(IF(RIGHT(Sheet1!B136, 1) = ".", LEFT(Sheet1!B136, LEN(Sheet1!B136)-1),Sheet1!B136))</f>
+        <v>0</v>
+      </c>
+      <c r="H136" t="b">
+        <f>TRIM(C136)=TRIM(IF(RIGHT(Sheet1!C136, 1) = ".", LEFT(Sheet1!C136, LEN(Sheet1!C136)-1),Sheet1!C136))</f>
+        <v>0</v>
+      </c>
+      <c r="I136" t="b">
+        <f>TRIM(D136)=TRIM(IF(RIGHT(Sheet1!D136, 1) = ".", LEFT(Sheet1!D136, LEN(Sheet1!D136)-1),Sheet1!D136))</f>
+        <v>0</v>
+      </c>
+      <c r="J136" t="b">
+        <f>TRIM(E136)=TRIM(IF(RIGHT(Sheet1!E136, 1) = ".", LEFT(Sheet1!E136, LEN(Sheet1!E136)-1),Sheet1!E136))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G137" t="b">
+        <f>TRIM(B137)=TRIM(IF(RIGHT(Sheet1!B137, 1) = ".", LEFT(Sheet1!B137, LEN(Sheet1!B137)-1),Sheet1!B137))</f>
+        <v>0</v>
+      </c>
+      <c r="H137" t="b">
+        <f>TRIM(C137)=TRIM(IF(RIGHT(Sheet1!C137, 1) = ".", LEFT(Sheet1!C137, LEN(Sheet1!C137)-1),Sheet1!C137))</f>
+        <v>0</v>
+      </c>
+      <c r="I137" t="b">
+        <f>TRIM(D137)=TRIM(IF(RIGHT(Sheet1!D137, 1) = ".", LEFT(Sheet1!D137, LEN(Sheet1!D137)-1),Sheet1!D137))</f>
+        <v>0</v>
+      </c>
+      <c r="J137" t="b">
+        <f>TRIM(E137)=TRIM(IF(RIGHT(Sheet1!E137, 1) = ".", LEFT(Sheet1!E137, LEN(Sheet1!E137)-1),Sheet1!E137))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G138" t="b">
+        <f>TRIM(B138)=TRIM(IF(RIGHT(Sheet1!B138, 1) = ".", LEFT(Sheet1!B138, LEN(Sheet1!B138)-1),Sheet1!B138))</f>
+        <v>0</v>
+      </c>
+      <c r="H138" t="b">
+        <f>TRIM(C138)=TRIM(IF(RIGHT(Sheet1!C138, 1) = ".", LEFT(Sheet1!C138, LEN(Sheet1!C138)-1),Sheet1!C138))</f>
+        <v>0</v>
+      </c>
+      <c r="I138" t="b">
+        <f>TRIM(D138)=TRIM(IF(RIGHT(Sheet1!D138, 1) = ".", LEFT(Sheet1!D138, LEN(Sheet1!D138)-1),Sheet1!D138))</f>
+        <v>0</v>
+      </c>
+      <c r="J138" t="b">
+        <f>TRIM(E138)=TRIM(IF(RIGHT(Sheet1!E138, 1) = ".", LEFT(Sheet1!E138, LEN(Sheet1!E138)-1),Sheet1!E138))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G139" t="b">
+        <f>TRIM(B139)=TRIM(IF(RIGHT(Sheet1!B139, 1) = ".", LEFT(Sheet1!B139, LEN(Sheet1!B139)-1),Sheet1!B139))</f>
+        <v>0</v>
+      </c>
+      <c r="H139" t="b">
+        <f>TRIM(C139)=TRIM(IF(RIGHT(Sheet1!C139, 1) = ".", LEFT(Sheet1!C139, LEN(Sheet1!C139)-1),Sheet1!C139))</f>
+        <v>0</v>
+      </c>
+      <c r="I139" t="b">
+        <f>TRIM(D139)=TRIM(IF(RIGHT(Sheet1!D139, 1) = ".", LEFT(Sheet1!D139, LEN(Sheet1!D139)-1),Sheet1!D139))</f>
+        <v>0</v>
+      </c>
+      <c r="J139" t="b">
+        <f>TRIM(E139)=TRIM(IF(RIGHT(Sheet1!E139, 1) = ".", LEFT(Sheet1!E139, LEN(Sheet1!E139)-1),Sheet1!E139))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G140" t="b">
+        <f>TRIM(B140)=TRIM(IF(RIGHT(Sheet1!B140, 1) = ".", LEFT(Sheet1!B140, LEN(Sheet1!B140)-1),Sheet1!B140))</f>
+        <v>0</v>
+      </c>
+      <c r="H140" t="b">
+        <f>TRIM(C140)=TRIM(IF(RIGHT(Sheet1!C140, 1) = ".", LEFT(Sheet1!C140, LEN(Sheet1!C140)-1),Sheet1!C140))</f>
+        <v>0</v>
+      </c>
+      <c r="I140" t="b">
+        <f>TRIM(D140)=TRIM(IF(RIGHT(Sheet1!D140, 1) = ".", LEFT(Sheet1!D140, LEN(Sheet1!D140)-1),Sheet1!D140))</f>
+        <v>0</v>
+      </c>
+      <c r="J140" t="b">
+        <f>TRIM(E140)=TRIM(IF(RIGHT(Sheet1!E140, 1) = ".", LEFT(Sheet1!E140, LEN(Sheet1!E140)-1),Sheet1!E140))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G141" t="b">
+        <f>TRIM(B141)=TRIM(IF(RIGHT(Sheet1!B141, 1) = ".", LEFT(Sheet1!B141, LEN(Sheet1!B141)-1),Sheet1!B141))</f>
+        <v>0</v>
+      </c>
+      <c r="H141" t="b">
+        <f>TRIM(C141)=TRIM(IF(RIGHT(Sheet1!C141, 1) = ".", LEFT(Sheet1!C141, LEN(Sheet1!C141)-1),Sheet1!C141))</f>
+        <v>0</v>
+      </c>
+      <c r="I141" t="b">
+        <f>TRIM(D141)=TRIM(IF(RIGHT(Sheet1!D141, 1) = ".", LEFT(Sheet1!D141, LEN(Sheet1!D141)-1),Sheet1!D141))</f>
+        <v>0</v>
+      </c>
+      <c r="J141" t="b">
+        <f>TRIM(E141)=TRIM(IF(RIGHT(Sheet1!E141, 1) = ".", LEFT(Sheet1!E141, LEN(Sheet1!E141)-1),Sheet1!E141))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G142" t="b">
+        <f>TRIM(B142)=TRIM(IF(RIGHT(Sheet1!B142, 1) = ".", LEFT(Sheet1!B142, LEN(Sheet1!B142)-1),Sheet1!B142))</f>
+        <v>0</v>
+      </c>
+      <c r="H142" t="b">
+        <f>TRIM(C142)=TRIM(IF(RIGHT(Sheet1!C142, 1) = ".", LEFT(Sheet1!C142, LEN(Sheet1!C142)-1),Sheet1!C142))</f>
+        <v>0</v>
+      </c>
+      <c r="I142" t="b">
+        <f>TRIM(D142)=TRIM(IF(RIGHT(Sheet1!D142, 1) = ".", LEFT(Sheet1!D142, LEN(Sheet1!D142)-1),Sheet1!D142))</f>
+        <v>0</v>
+      </c>
+      <c r="J142" t="b">
+        <f>TRIM(E142)=TRIM(IF(RIGHT(Sheet1!E142, 1) = ".", LEFT(Sheet1!E142, LEN(Sheet1!E142)-1),Sheet1!E142))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G143" t="b">
+        <f>TRIM(B143)=TRIM(IF(RIGHT(Sheet1!B143, 1) = ".", LEFT(Sheet1!B143, LEN(Sheet1!B143)-1),Sheet1!B143))</f>
+        <v>0</v>
+      </c>
+      <c r="H143" t="b">
+        <f>TRIM(C143)=TRIM(IF(RIGHT(Sheet1!C143, 1) = ".", LEFT(Sheet1!C143, LEN(Sheet1!C143)-1),Sheet1!C143))</f>
+        <v>0</v>
+      </c>
+      <c r="I143" t="b">
+        <f>TRIM(D143)=TRIM(IF(RIGHT(Sheet1!D143, 1) = ".", LEFT(Sheet1!D143, LEN(Sheet1!D143)-1),Sheet1!D143))</f>
+        <v>0</v>
+      </c>
+      <c r="J143" t="b">
+        <f>TRIM(E143)=TRIM(IF(RIGHT(Sheet1!E143, 1) = ".", LEFT(Sheet1!E143, LEN(Sheet1!E143)-1),Sheet1!E143))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G144" t="b">
+        <f>TRIM(B144)=TRIM(IF(RIGHT(Sheet1!B144, 1) = ".", LEFT(Sheet1!B144, LEN(Sheet1!B144)-1),Sheet1!B144))</f>
+        <v>0</v>
+      </c>
+      <c r="H144" t="b">
+        <f>TRIM(C144)=TRIM(IF(RIGHT(Sheet1!C144, 1) = ".", LEFT(Sheet1!C144, LEN(Sheet1!C144)-1),Sheet1!C144))</f>
+        <v>0</v>
+      </c>
+      <c r="I144" t="b">
+        <f>TRIM(D144)=TRIM(IF(RIGHT(Sheet1!D144, 1) = ".", LEFT(Sheet1!D144, LEN(Sheet1!D144)-1),Sheet1!D144))</f>
+        <v>0</v>
+      </c>
+      <c r="J144" t="b">
+        <f>TRIM(E144)=TRIM(IF(RIGHT(Sheet1!E144, 1) = ".", LEFT(Sheet1!E144, LEN(Sheet1!E144)-1),Sheet1!E144))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G145" t="b">
+        <f>TRIM(B145)=TRIM(IF(RIGHT(Sheet1!B145, 1) = ".", LEFT(Sheet1!B145, LEN(Sheet1!B145)-1),Sheet1!B145))</f>
+        <v>0</v>
+      </c>
+      <c r="H145" t="b">
+        <f>TRIM(C145)=TRIM(IF(RIGHT(Sheet1!C145, 1) = ".", LEFT(Sheet1!C145, LEN(Sheet1!C145)-1),Sheet1!C145))</f>
+        <v>0</v>
+      </c>
+      <c r="I145" t="b">
+        <f>TRIM(D145)=TRIM(IF(RIGHT(Sheet1!D145, 1) = ".", LEFT(Sheet1!D145, LEN(Sheet1!D145)-1),Sheet1!D145))</f>
+        <v>0</v>
+      </c>
+      <c r="J145" t="b">
+        <f>TRIM(E145)=TRIM(IF(RIGHT(Sheet1!E145, 1) = ".", LEFT(Sheet1!E145, LEN(Sheet1!E145)-1),Sheet1!E145))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G146" t="b">
+        <f>TRIM(B146)=TRIM(IF(RIGHT(Sheet1!B146, 1) = ".", LEFT(Sheet1!B146, LEN(Sheet1!B146)-1),Sheet1!B146))</f>
+        <v>0</v>
+      </c>
+      <c r="H146" t="b">
+        <f>TRIM(C146)=TRIM(IF(RIGHT(Sheet1!C146, 1) = ".", LEFT(Sheet1!C146, LEN(Sheet1!C146)-1),Sheet1!C146))</f>
+        <v>0</v>
+      </c>
+      <c r="I146" t="b">
+        <f>TRIM(D146)=TRIM(IF(RIGHT(Sheet1!D146, 1) = ".", LEFT(Sheet1!D146, LEN(Sheet1!D146)-1),Sheet1!D146))</f>
+        <v>0</v>
+      </c>
+      <c r="J146" t="b">
+        <f>TRIM(E146)=TRIM(IF(RIGHT(Sheet1!E146, 1) = ".", LEFT(Sheet1!E146, LEN(Sheet1!E146)-1),Sheet1!E146))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G147" t="b">
+        <f>TRIM(B147)=TRIM(IF(RIGHT(Sheet1!B147, 1) = ".", LEFT(Sheet1!B147, LEN(Sheet1!B147)-1),Sheet1!B147))</f>
+        <v>0</v>
+      </c>
+      <c r="H147" t="b">
+        <f>TRIM(C147)=TRIM(IF(RIGHT(Sheet1!C147, 1) = ".", LEFT(Sheet1!C147, LEN(Sheet1!C147)-1),Sheet1!C147))</f>
+        <v>0</v>
+      </c>
+      <c r="I147" t="b">
+        <f>TRIM(D147)=TRIM(IF(RIGHT(Sheet1!D147, 1) = ".", LEFT(Sheet1!D147, LEN(Sheet1!D147)-1),Sheet1!D147))</f>
+        <v>0</v>
+      </c>
+      <c r="J147" t="b">
+        <f>TRIM(E147)=TRIM(IF(RIGHT(Sheet1!E147, 1) = ".", LEFT(Sheet1!E147, LEN(Sheet1!E147)-1),Sheet1!E147))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G148" t="b">
+        <f>TRIM(B148)=TRIM(IF(RIGHT(Sheet1!B148, 1) = ".", LEFT(Sheet1!B148, LEN(Sheet1!B148)-1),Sheet1!B148))</f>
+        <v>0</v>
+      </c>
+      <c r="H148" t="b">
+        <f>TRIM(C148)=TRIM(IF(RIGHT(Sheet1!C148, 1) = ".", LEFT(Sheet1!C148, LEN(Sheet1!C148)-1),Sheet1!C148))</f>
+        <v>0</v>
+      </c>
+      <c r="I148" t="b">
+        <f>TRIM(D148)=TRIM(IF(RIGHT(Sheet1!D148, 1) = ".", LEFT(Sheet1!D148, LEN(Sheet1!D148)-1),Sheet1!D148))</f>
+        <v>0</v>
+      </c>
+      <c r="J148" t="b">
+        <f>TRIM(E148)=TRIM(IF(RIGHT(Sheet1!E148, 1) = ".", LEFT(Sheet1!E148, LEN(Sheet1!E148)-1),Sheet1!E148))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G149" t="b">
+        <f>TRIM(B149)=TRIM(IF(RIGHT(Sheet1!B149, 1) = ".", LEFT(Sheet1!B149, LEN(Sheet1!B149)-1),Sheet1!B149))</f>
+        <v>0</v>
+      </c>
+      <c r="H149" t="b">
+        <f>TRIM(C149)=TRIM(IF(RIGHT(Sheet1!C149, 1) = ".", LEFT(Sheet1!C149, LEN(Sheet1!C149)-1),Sheet1!C149))</f>
+        <v>0</v>
+      </c>
+      <c r="I149" t="b">
+        <f>TRIM(D149)=TRIM(IF(RIGHT(Sheet1!D149, 1) = ".", LEFT(Sheet1!D149, LEN(Sheet1!D149)-1),Sheet1!D149))</f>
+        <v>0</v>
+      </c>
+      <c r="J149" t="b">
+        <f>TRIM(E149)=TRIM(IF(RIGHT(Sheet1!E149, 1) = ".", LEFT(Sheet1!E149, LEN(Sheet1!E149)-1),Sheet1!E149))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G150" t="b">
+        <f>TRIM(B150)=TRIM(IF(RIGHT(Sheet1!B150, 1) = ".", LEFT(Sheet1!B150, LEN(Sheet1!B150)-1),Sheet1!B150))</f>
+        <v>0</v>
+      </c>
+      <c r="H150" t="b">
+        <f>TRIM(C150)=TRIM(IF(RIGHT(Sheet1!C150, 1) = ".", LEFT(Sheet1!C150, LEN(Sheet1!C150)-1),Sheet1!C150))</f>
+        <v>0</v>
+      </c>
+      <c r="I150" t="b">
+        <f>TRIM(D150)=TRIM(IF(RIGHT(Sheet1!D150, 1) = ".", LEFT(Sheet1!D150, LEN(Sheet1!D150)-1),Sheet1!D150))</f>
+        <v>0</v>
+      </c>
+      <c r="J150" t="b">
+        <f>TRIM(E150)=TRIM(IF(RIGHT(Sheet1!E150, 1) = ".", LEFT(Sheet1!E150, LEN(Sheet1!E150)-1),Sheet1!E150))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G151" t="b">
+        <f>TRIM(B151)=TRIM(IF(RIGHT(Sheet1!B151, 1) = ".", LEFT(Sheet1!B151, LEN(Sheet1!B151)-1),Sheet1!B151))</f>
+        <v>0</v>
+      </c>
+      <c r="H151" t="b">
+        <f>TRIM(C151)=TRIM(IF(RIGHT(Sheet1!C151, 1) = ".", LEFT(Sheet1!C151, LEN(Sheet1!C151)-1),Sheet1!C151))</f>
+        <v>0</v>
+      </c>
+      <c r="I151" t="b">
+        <f>TRIM(D151)=TRIM(IF(RIGHT(Sheet1!D151, 1) = ".", LEFT(Sheet1!D151, LEN(Sheet1!D151)-1),Sheet1!D151))</f>
+        <v>0</v>
+      </c>
+      <c r="J151" t="b">
+        <f>TRIM(E151)=TRIM(IF(RIGHT(Sheet1!E151, 1) = ".", LEFT(Sheet1!E151, LEN(Sheet1!E151)-1),Sheet1!E151))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G152" t="b">
+        <f>TRIM(B152)=TRIM(IF(RIGHT(Sheet1!B152, 1) = ".", LEFT(Sheet1!B152, LEN(Sheet1!B152)-1),Sheet1!B152))</f>
+        <v>0</v>
+      </c>
+      <c r="H152" t="b">
+        <f>TRIM(C152)=TRIM(IF(RIGHT(Sheet1!C152, 1) = ".", LEFT(Sheet1!C152, LEN(Sheet1!C152)-1),Sheet1!C152))</f>
+        <v>0</v>
+      </c>
+      <c r="I152" t="b">
+        <f>TRIM(D152)=TRIM(IF(RIGHT(Sheet1!D152, 1) = ".", LEFT(Sheet1!D152, LEN(Sheet1!D152)-1),Sheet1!D152))</f>
+        <v>0</v>
+      </c>
+      <c r="J152" t="b">
+        <f>TRIM(E152)=TRIM(IF(RIGHT(Sheet1!E152, 1) = ".", LEFT(Sheet1!E152, LEN(Sheet1!E152)-1),Sheet1!E152))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G153" t="b">
+        <f>TRIM(B153)=TRIM(IF(RIGHT(Sheet1!B153, 1) = ".", LEFT(Sheet1!B153, LEN(Sheet1!B153)-1),Sheet1!B153))</f>
+        <v>0</v>
+      </c>
+      <c r="H153" t="b">
+        <f>TRIM(C153)=TRIM(IF(RIGHT(Sheet1!C153, 1) = ".", LEFT(Sheet1!C153, LEN(Sheet1!C153)-1),Sheet1!C153))</f>
+        <v>0</v>
+      </c>
+      <c r="I153" t="b">
+        <f>TRIM(D153)=TRIM(IF(RIGHT(Sheet1!D153, 1) = ".", LEFT(Sheet1!D153, LEN(Sheet1!D153)-1),Sheet1!D153))</f>
+        <v>0</v>
+      </c>
+      <c r="J153" t="b">
+        <f>TRIM(E153)=TRIM(IF(RIGHT(Sheet1!E153, 1) = ".", LEFT(Sheet1!E153, LEN(Sheet1!E153)-1),Sheet1!E153))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G154" t="b">
+        <f>TRIM(B154)=TRIM(IF(RIGHT(Sheet1!B154, 1) = ".", LEFT(Sheet1!B154, LEN(Sheet1!B154)-1),Sheet1!B154))</f>
+        <v>0</v>
+      </c>
+      <c r="H154" t="b">
+        <f>TRIM(C154)=TRIM(IF(RIGHT(Sheet1!C154, 1) = ".", LEFT(Sheet1!C154, LEN(Sheet1!C154)-1),Sheet1!C154))</f>
+        <v>0</v>
+      </c>
+      <c r="I154" t="b">
+        <f>TRIM(D154)=TRIM(IF(RIGHT(Sheet1!D154, 1) = ".", LEFT(Sheet1!D154, LEN(Sheet1!D154)-1),Sheet1!D154))</f>
+        <v>0</v>
+      </c>
+      <c r="J154" t="b">
+        <f>TRIM(E154)=TRIM(IF(RIGHT(Sheet1!E154, 1) = ".", LEFT(Sheet1!E154, LEN(Sheet1!E154)-1),Sheet1!E154))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G155" t="b">
+        <f>TRIM(B155)=TRIM(IF(RIGHT(Sheet1!B155, 1) = ".", LEFT(Sheet1!B155, LEN(Sheet1!B155)-1),Sheet1!B155))</f>
+        <v>0</v>
+      </c>
+      <c r="H155" t="b">
+        <f>TRIM(C155)=TRIM(IF(RIGHT(Sheet1!C155, 1) = ".", LEFT(Sheet1!C155, LEN(Sheet1!C155)-1),Sheet1!C155))</f>
+        <v>0</v>
+      </c>
+      <c r="I155" t="b">
+        <f>TRIM(D155)=TRIM(IF(RIGHT(Sheet1!D155, 1) = ".", LEFT(Sheet1!D155, LEN(Sheet1!D155)-1),Sheet1!D155))</f>
+        <v>0</v>
+      </c>
+      <c r="J155" t="b">
+        <f>TRIM(E155)=TRIM(IF(RIGHT(Sheet1!E155, 1) = ".", LEFT(Sheet1!E155, LEN(Sheet1!E155)-1),Sheet1!E155))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G156" t="b">
+        <f>TRIM(B156)=TRIM(IF(RIGHT(Sheet1!B156, 1) = ".", LEFT(Sheet1!B156, LEN(Sheet1!B156)-1),Sheet1!B156))</f>
+        <v>0</v>
+      </c>
+      <c r="H156" t="b">
+        <f>TRIM(C156)=TRIM(IF(RIGHT(Sheet1!C156, 1) = ".", LEFT(Sheet1!C156, LEN(Sheet1!C156)-1),Sheet1!C156))</f>
+        <v>0</v>
+      </c>
+      <c r="I156" t="b">
+        <f>TRIM(D156)=TRIM(IF(RIGHT(Sheet1!D156, 1) = ".", LEFT(Sheet1!D156, LEN(Sheet1!D156)-1),Sheet1!D156))</f>
+        <v>0</v>
+      </c>
+      <c r="J156" t="b">
+        <f>TRIM(E156)=TRIM(IF(RIGHT(Sheet1!E156, 1) = ".", LEFT(Sheet1!E156, LEN(Sheet1!E156)-1),Sheet1!E156))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G157" t="b">
+        <f>TRIM(B157)=TRIM(IF(RIGHT(Sheet1!B157, 1) = ".", LEFT(Sheet1!B157, LEN(Sheet1!B157)-1),Sheet1!B157))</f>
+        <v>0</v>
+      </c>
+      <c r="H157" t="b">
+        <f>TRIM(C157)=TRIM(IF(RIGHT(Sheet1!C157, 1) = ".", LEFT(Sheet1!C157, LEN(Sheet1!C157)-1),Sheet1!C157))</f>
+        <v>0</v>
+      </c>
+      <c r="I157" t="b">
+        <f>TRIM(D157)=TRIM(IF(RIGHT(Sheet1!D157, 1) = ".", LEFT(Sheet1!D157, LEN(Sheet1!D157)-1),Sheet1!D157))</f>
+        <v>0</v>
+      </c>
+      <c r="J157" t="b">
+        <f>TRIM(E157)=TRIM(IF(RIGHT(Sheet1!E157, 1) = ".", LEFT(Sheet1!E157, LEN(Sheet1!E157)-1),Sheet1!E157))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G158" t="b">
+        <f>TRIM(B158)=TRIM(IF(RIGHT(Sheet1!B158, 1) = ".", LEFT(Sheet1!B158, LEN(Sheet1!B158)-1),Sheet1!B158))</f>
+        <v>0</v>
+      </c>
+      <c r="H158" t="b">
+        <f>TRIM(C158)=TRIM(IF(RIGHT(Sheet1!C158, 1) = ".", LEFT(Sheet1!C158, LEN(Sheet1!C158)-1),Sheet1!C158))</f>
+        <v>0</v>
+      </c>
+      <c r="I158" t="b">
+        <f>TRIM(D158)=TRIM(IF(RIGHT(Sheet1!D158, 1) = ".", LEFT(Sheet1!D158, LEN(Sheet1!D158)-1),Sheet1!D158))</f>
+        <v>0</v>
+      </c>
+      <c r="J158" t="b">
+        <f>TRIM(E158)=TRIM(IF(RIGHT(Sheet1!E158, 1) = ".", LEFT(Sheet1!E158, LEN(Sheet1!E158)-1),Sheet1!E158))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G159" t="b">
+        <f>TRIM(B159)=TRIM(IF(RIGHT(Sheet1!B159, 1) = ".", LEFT(Sheet1!B159, LEN(Sheet1!B159)-1),Sheet1!B159))</f>
+        <v>0</v>
+      </c>
+      <c r="H159" t="b">
+        <f>TRIM(C159)=TRIM(IF(RIGHT(Sheet1!C159, 1) = ".", LEFT(Sheet1!C159, LEN(Sheet1!C159)-1),Sheet1!C159))</f>
+        <v>0</v>
+      </c>
+      <c r="I159" t="b">
+        <f>TRIM(D159)=TRIM(IF(RIGHT(Sheet1!D159, 1) = ".", LEFT(Sheet1!D159, LEN(Sheet1!D159)-1),Sheet1!D159))</f>
+        <v>0</v>
+      </c>
+      <c r="J159" t="b">
+        <f>TRIM(E159)=TRIM(IF(RIGHT(Sheet1!E159, 1) = ".", LEFT(Sheet1!E159, LEN(Sheet1!E159)-1),Sheet1!E159))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G160" t="b">
+        <f>TRIM(B160)=TRIM(IF(RIGHT(Sheet1!B160, 1) = ".", LEFT(Sheet1!B160, LEN(Sheet1!B160)-1),Sheet1!B160))</f>
+        <v>0</v>
+      </c>
+      <c r="H160" t="b">
+        <f>TRIM(C160)=TRIM(IF(RIGHT(Sheet1!C160, 1) = ".", LEFT(Sheet1!C160, LEN(Sheet1!C160)-1),Sheet1!C160))</f>
+        <v>0</v>
+      </c>
+      <c r="I160" t="b">
+        <f>TRIM(D160)=TRIM(IF(RIGHT(Sheet1!D160, 1) = ".", LEFT(Sheet1!D160, LEN(Sheet1!D160)-1),Sheet1!D160))</f>
+        <v>0</v>
+      </c>
+      <c r="J160" t="b">
+        <f>TRIM(E160)=TRIM(IF(RIGHT(Sheet1!E160, 1) = ".", LEFT(Sheet1!E160, LEN(Sheet1!E160)-1),Sheet1!E160))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G161" t="b">
+        <f>TRIM(B161)=TRIM(IF(RIGHT(Sheet1!B161, 1) = ".", LEFT(Sheet1!B161, LEN(Sheet1!B161)-1),Sheet1!B161))</f>
+        <v>0</v>
+      </c>
+      <c r="H161" t="b">
+        <f>TRIM(C161)=TRIM(IF(RIGHT(Sheet1!C161, 1) = ".", LEFT(Sheet1!C161, LEN(Sheet1!C161)-1),Sheet1!C161))</f>
+        <v>0</v>
+      </c>
+      <c r="I161" t="b">
+        <f>TRIM(D161)=TRIM(IF(RIGHT(Sheet1!D161, 1) = ".", LEFT(Sheet1!D161, LEN(Sheet1!D161)-1),Sheet1!D161))</f>
+        <v>0</v>
+      </c>
+      <c r="J161" t="b">
+        <f>TRIM(E161)=TRIM(IF(RIGHT(Sheet1!E161, 1) = ".", LEFT(Sheet1!E161, LEN(Sheet1!E161)-1),Sheet1!E161))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G162" t="b">
+        <f>TRIM(B162)=TRIM(IF(RIGHT(Sheet1!B162, 1) = ".", LEFT(Sheet1!B162, LEN(Sheet1!B162)-1),Sheet1!B162))</f>
+        <v>0</v>
+      </c>
+      <c r="H162" t="b">
+        <f>TRIM(C162)=TRIM(IF(RIGHT(Sheet1!C162, 1) = ".", LEFT(Sheet1!C162, LEN(Sheet1!C162)-1),Sheet1!C162))</f>
+        <v>0</v>
+      </c>
+      <c r="I162" t="b">
+        <f>TRIM(D162)=TRIM(IF(RIGHT(Sheet1!D162, 1) = ".", LEFT(Sheet1!D162, LEN(Sheet1!D162)-1),Sheet1!D162))</f>
+        <v>0</v>
+      </c>
+      <c r="J162" t="b">
+        <f>TRIM(E162)=TRIM(IF(RIGHT(Sheet1!E162, 1) = ".", LEFT(Sheet1!E162, LEN(Sheet1!E162)-1),Sheet1!E162))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G163" t="b">
+        <f>TRIM(B163)=TRIM(IF(RIGHT(Sheet1!B163, 1) = ".", LEFT(Sheet1!B163, LEN(Sheet1!B163)-1),Sheet1!B163))</f>
+        <v>0</v>
+      </c>
+      <c r="H163" t="b">
+        <f>TRIM(C163)=TRIM(IF(RIGHT(Sheet1!C163, 1) = ".", LEFT(Sheet1!C163, LEN(Sheet1!C163)-1),Sheet1!C163))</f>
+        <v>0</v>
+      </c>
+      <c r="I163" t="b">
+        <f>TRIM(D163)=TRIM(IF(RIGHT(Sheet1!D163, 1) = ".", LEFT(Sheet1!D163, LEN(Sheet1!D163)-1),Sheet1!D163))</f>
+        <v>0</v>
+      </c>
+      <c r="J163" t="b">
+        <f>TRIM(E163)=TRIM(IF(RIGHT(Sheet1!E163, 1) = ".", LEFT(Sheet1!E163, LEN(Sheet1!E163)-1),Sheet1!E163))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G164" t="b">
+        <f>TRIM(B164)=TRIM(IF(RIGHT(Sheet1!B164, 1) = ".", LEFT(Sheet1!B164, LEN(Sheet1!B164)-1),Sheet1!B164))</f>
+        <v>0</v>
+      </c>
+      <c r="H164" t="b">
+        <f>TRIM(C164)=TRIM(IF(RIGHT(Sheet1!C164, 1) = ".", LEFT(Sheet1!C164, LEN(Sheet1!C164)-1),Sheet1!C164))</f>
+        <v>0</v>
+      </c>
+      <c r="I164" t="b">
+        <f>TRIM(D164)=TRIM(IF(RIGHT(Sheet1!D164, 1) = ".", LEFT(Sheet1!D164, LEN(Sheet1!D164)-1),Sheet1!D164))</f>
+        <v>0</v>
+      </c>
+      <c r="J164" t="b">
+        <f>TRIM(E164)=TRIM(IF(RIGHT(Sheet1!E164, 1) = ".", LEFT(Sheet1!E164, LEN(Sheet1!E164)-1),Sheet1!E164))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G165" t="b">
+        <f>TRIM(B165)=TRIM(IF(RIGHT(Sheet1!B165, 1) = ".", LEFT(Sheet1!B165, LEN(Sheet1!B165)-1),Sheet1!B165))</f>
+        <v>0</v>
+      </c>
+      <c r="H165" t="b">
+        <f>TRIM(C165)=TRIM(IF(RIGHT(Sheet1!C165, 1) = ".", LEFT(Sheet1!C165, LEN(Sheet1!C165)-1),Sheet1!C165))</f>
+        <v>0</v>
+      </c>
+      <c r="I165" t="b">
+        <f>TRIM(D165)=TRIM(IF(RIGHT(Sheet1!D165, 1) = ".", LEFT(Sheet1!D165, LEN(Sheet1!D165)-1),Sheet1!D165))</f>
+        <v>0</v>
+      </c>
+      <c r="J165" t="b">
+        <f>TRIM(E165)=TRIM(IF(RIGHT(Sheet1!E165, 1) = ".", LEFT(Sheet1!E165, LEN(Sheet1!E165)-1),Sheet1!E165))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G166" t="b">
+        <f>TRIM(B166)=TRIM(IF(RIGHT(Sheet1!B166, 1) = ".", LEFT(Sheet1!B166, LEN(Sheet1!B166)-1),Sheet1!B166))</f>
+        <v>0</v>
+      </c>
+      <c r="H166" t="b">
+        <f>TRIM(C166)=TRIM(IF(RIGHT(Sheet1!C166, 1) = ".", LEFT(Sheet1!C166, LEN(Sheet1!C166)-1),Sheet1!C166))</f>
+        <v>0</v>
+      </c>
+      <c r="I166" t="b">
+        <f>TRIM(D166)=TRIM(IF(RIGHT(Sheet1!D166, 1) = ".", LEFT(Sheet1!D166, LEN(Sheet1!D166)-1),Sheet1!D166))</f>
+        <v>0</v>
+      </c>
+      <c r="J166" t="b">
+        <f>TRIM(E166)=TRIM(IF(RIGHT(Sheet1!E166, 1) = ".", LEFT(Sheet1!E166, LEN(Sheet1!E166)-1),Sheet1!E166))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G167" t="b">
+        <f>TRIM(B167)=TRIM(IF(RIGHT(Sheet1!B167, 1) = ".", LEFT(Sheet1!B167, LEN(Sheet1!B167)-1),Sheet1!B167))</f>
+        <v>0</v>
+      </c>
+      <c r="H167" t="b">
+        <f>TRIM(C167)=TRIM(IF(RIGHT(Sheet1!C167, 1) = ".", LEFT(Sheet1!C167, LEN(Sheet1!C167)-1),Sheet1!C167))</f>
+        <v>0</v>
+      </c>
+      <c r="I167" t="b">
+        <f>TRIM(D167)=TRIM(IF(RIGHT(Sheet1!D167, 1) = ".", LEFT(Sheet1!D167, LEN(Sheet1!D167)-1),Sheet1!D167))</f>
+        <v>0</v>
+      </c>
+      <c r="J167" t="b">
+        <f>TRIM(E167)=TRIM(IF(RIGHT(Sheet1!E167, 1) = ".", LEFT(Sheet1!E167, LEN(Sheet1!E167)-1),Sheet1!E167))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G168" t="b">
+        <f>TRIM(B168)=TRIM(IF(RIGHT(Sheet1!B168, 1) = ".", LEFT(Sheet1!B168, LEN(Sheet1!B168)-1),Sheet1!B168))</f>
+        <v>0</v>
+      </c>
+      <c r="H168" t="b">
+        <f>TRIM(C168)=TRIM(IF(RIGHT(Sheet1!C168, 1) = ".", LEFT(Sheet1!C168, LEN(Sheet1!C168)-1),Sheet1!C168))</f>
+        <v>0</v>
+      </c>
+      <c r="I168" t="b">
+        <f>TRIM(D168)=TRIM(IF(RIGHT(Sheet1!D168, 1) = ".", LEFT(Sheet1!D168, LEN(Sheet1!D168)-1),Sheet1!D168))</f>
+        <v>0</v>
+      </c>
+      <c r="J168" t="b">
+        <f>TRIM(E168)=TRIM(IF(RIGHT(Sheet1!E168, 1) = ".", LEFT(Sheet1!E168, LEN(Sheet1!E168)-1),Sheet1!E168))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G169" t="b">
+        <f>TRIM(B169)=TRIM(IF(RIGHT(Sheet1!B169, 1) = ".", LEFT(Sheet1!B169, LEN(Sheet1!B169)-1),Sheet1!B169))</f>
+        <v>0</v>
+      </c>
+      <c r="H169" t="b">
+        <f>TRIM(C169)=TRIM(IF(RIGHT(Sheet1!C169, 1) = ".", LEFT(Sheet1!C169, LEN(Sheet1!C169)-1),Sheet1!C169))</f>
+        <v>0</v>
+      </c>
+      <c r="I169" t="b">
+        <f>TRIM(D169)=TRIM(IF(RIGHT(Sheet1!D169, 1) = ".", LEFT(Sheet1!D169, LEN(Sheet1!D169)-1),Sheet1!D169))</f>
+        <v>0</v>
+      </c>
+      <c r="J169" t="b">
+        <f>TRIM(E169)=TRIM(IF(RIGHT(Sheet1!E169, 1) = ".", LEFT(Sheet1!E169, LEN(Sheet1!E169)-1),Sheet1!E169))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G170" t="b">
+        <f>TRIM(B170)=TRIM(IF(RIGHT(Sheet1!B170, 1) = ".", LEFT(Sheet1!B170, LEN(Sheet1!B170)-1),Sheet1!B170))</f>
+        <v>0</v>
+      </c>
+      <c r="H170" t="b">
+        <f>TRIM(C170)=TRIM(IF(RIGHT(Sheet1!C170, 1) = ".", LEFT(Sheet1!C170, LEN(Sheet1!C170)-1),Sheet1!C170))</f>
+        <v>0</v>
+      </c>
+      <c r="I170" t="b">
+        <f>TRIM(D170)=TRIM(IF(RIGHT(Sheet1!D170, 1) = ".", LEFT(Sheet1!D170, LEN(Sheet1!D170)-1),Sheet1!D170))</f>
+        <v>0</v>
+      </c>
+      <c r="J170" t="b">
+        <f>TRIM(E170)=TRIM(IF(RIGHT(Sheet1!E170, 1) = ".", LEFT(Sheet1!E170, LEN(Sheet1!E170)-1),Sheet1!E170))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G171" t="b">
+        <f>TRIM(B171)=TRIM(IF(RIGHT(Sheet1!B171, 1) = ".", LEFT(Sheet1!B171, LEN(Sheet1!B171)-1),Sheet1!B171))</f>
+        <v>0</v>
+      </c>
+      <c r="H171" t="b">
+        <f>TRIM(C171)=TRIM(IF(RIGHT(Sheet1!C171, 1) = ".", LEFT(Sheet1!C171, LEN(Sheet1!C171)-1),Sheet1!C171))</f>
+        <v>0</v>
+      </c>
+      <c r="I171" t="b">
+        <f>TRIM(D171)=TRIM(IF(RIGHT(Sheet1!D171, 1) = ".", LEFT(Sheet1!D171, LEN(Sheet1!D171)-1),Sheet1!D171))</f>
+        <v>0</v>
+      </c>
+      <c r="J171" t="b">
+        <f>TRIM(E171)=TRIM(IF(RIGHT(Sheet1!E171, 1) = ".", LEFT(Sheet1!E171, LEN(Sheet1!E171)-1),Sheet1!E171))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G172" t="b">
+        <f>TRIM(B172)=TRIM(IF(RIGHT(Sheet1!B172, 1) = ".", LEFT(Sheet1!B172, LEN(Sheet1!B172)-1),Sheet1!B172))</f>
+        <v>0</v>
+      </c>
+      <c r="H172" t="b">
+        <f>TRIM(C172)=TRIM(IF(RIGHT(Sheet1!C172, 1) = ".", LEFT(Sheet1!C172, LEN(Sheet1!C172)-1),Sheet1!C172))</f>
+        <v>0</v>
+      </c>
+      <c r="I172" t="b">
+        <f>TRIM(D172)=TRIM(IF(RIGHT(Sheet1!D172, 1) = ".", LEFT(Sheet1!D172, LEN(Sheet1!D172)-1),Sheet1!D172))</f>
+        <v>0</v>
+      </c>
+      <c r="J172" t="b">
+        <f>TRIM(E172)=TRIM(IF(RIGHT(Sheet1!E172, 1) = ".", LEFT(Sheet1!E172, LEN(Sheet1!E172)-1),Sheet1!E172))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G173" t="b">
+        <f>TRIM(B173)=TRIM(IF(RIGHT(Sheet1!B173, 1) = ".", LEFT(Sheet1!B173, LEN(Sheet1!B173)-1),Sheet1!B173))</f>
+        <v>0</v>
+      </c>
+      <c r="H173" t="b">
+        <f>TRIM(C173)=TRIM(IF(RIGHT(Sheet1!C173, 1) = ".", LEFT(Sheet1!C173, LEN(Sheet1!C173)-1),Sheet1!C173))</f>
+        <v>0</v>
+      </c>
+      <c r="I173" t="b">
+        <f>TRIM(D173)=TRIM(IF(RIGHT(Sheet1!D173, 1) = ".", LEFT(Sheet1!D173, LEN(Sheet1!D173)-1),Sheet1!D173))</f>
+        <v>0</v>
+      </c>
+      <c r="J173" t="b">
+        <f>TRIM(E173)=TRIM(IF(RIGHT(Sheet1!E173, 1) = ".", LEFT(Sheet1!E173, LEN(Sheet1!E173)-1),Sheet1!E173))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G174" t="b">
+        <f>TRIM(B174)=TRIM(IF(RIGHT(Sheet1!B174, 1) = ".", LEFT(Sheet1!B174, LEN(Sheet1!B174)-1),Sheet1!B174))</f>
+        <v>0</v>
+      </c>
+      <c r="H174" t="b">
+        <f>TRIM(C174)=TRIM(IF(RIGHT(Sheet1!C174, 1) = ".", LEFT(Sheet1!C174, LEN(Sheet1!C174)-1),Sheet1!C174))</f>
+        <v>0</v>
+      </c>
+      <c r="I174" t="b">
+        <f>TRIM(D174)=TRIM(IF(RIGHT(Sheet1!D174, 1) = ".", LEFT(Sheet1!D174, LEN(Sheet1!D174)-1),Sheet1!D174))</f>
+        <v>0</v>
+      </c>
+      <c r="J174" t="b">
+        <f>TRIM(E174)=TRIM(IF(RIGHT(Sheet1!E174, 1) = ".", LEFT(Sheet1!E174, LEN(Sheet1!E174)-1),Sheet1!E174))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G175" t="b">
+        <f>TRIM(B175)=TRIM(IF(RIGHT(Sheet1!B175, 1) = ".", LEFT(Sheet1!B175, LEN(Sheet1!B175)-1),Sheet1!B175))</f>
+        <v>0</v>
+      </c>
+      <c r="H175" t="b">
+        <f>TRIM(C175)=TRIM(IF(RIGHT(Sheet1!C175, 1) = ".", LEFT(Sheet1!C175, LEN(Sheet1!C175)-1),Sheet1!C175))</f>
+        <v>0</v>
+      </c>
+      <c r="I175" t="b">
+        <f>TRIM(D175)=TRIM(IF(RIGHT(Sheet1!D175, 1) = ".", LEFT(Sheet1!D175, LEN(Sheet1!D175)-1),Sheet1!D175))</f>
+        <v>0</v>
+      </c>
+      <c r="J175" t="b">
+        <f>TRIM(E175)=TRIM(IF(RIGHT(Sheet1!E175, 1) = ".", LEFT(Sheet1!E175, LEN(Sheet1!E175)-1),Sheet1!E175))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G176" t="b">
+        <f>TRIM(B176)=TRIM(IF(RIGHT(Sheet1!B176, 1) = ".", LEFT(Sheet1!B176, LEN(Sheet1!B176)-1),Sheet1!B176))</f>
+        <v>0</v>
+      </c>
+      <c r="H176" t="b">
+        <f>TRIM(C176)=TRIM(IF(RIGHT(Sheet1!C176, 1) = ".", LEFT(Sheet1!C176, LEN(Sheet1!C176)-1),Sheet1!C176))</f>
+        <v>0</v>
+      </c>
+      <c r="I176" t="b">
+        <f>TRIM(D176)=TRIM(IF(RIGHT(Sheet1!D176, 1) = ".", LEFT(Sheet1!D176, LEN(Sheet1!D176)-1),Sheet1!D176))</f>
+        <v>0</v>
+      </c>
+      <c r="J176" t="b">
+        <f>TRIM(E176)=TRIM(IF(RIGHT(Sheet1!E176, 1) = ".", LEFT(Sheet1!E176, LEN(Sheet1!E176)-1),Sheet1!E176))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G177" t="b">
+        <f>TRIM(B177)=TRIM(IF(RIGHT(Sheet1!B177, 1) = ".", LEFT(Sheet1!B177, LEN(Sheet1!B177)-1),Sheet1!B177))</f>
+        <v>0</v>
+      </c>
+      <c r="H177" t="b">
+        <f>TRIM(C177)=TRIM(IF(RIGHT(Sheet1!C177, 1) = ".", LEFT(Sheet1!C177, LEN(Sheet1!C177)-1),Sheet1!C177))</f>
+        <v>0</v>
+      </c>
+      <c r="I177" t="b">
+        <f>TRIM(D177)=TRIM(IF(RIGHT(Sheet1!D177, 1) = ".", LEFT(Sheet1!D177, LEN(Sheet1!D177)-1),Sheet1!D177))</f>
+        <v>0</v>
+      </c>
+      <c r="J177" t="b">
+        <f>TRIM(E177)=TRIM(IF(RIGHT(Sheet1!E177, 1) = ".", LEFT(Sheet1!E177, LEN(Sheet1!E177)-1),Sheet1!E177))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G178" t="b">
+        <f>TRIM(B178)=TRIM(IF(RIGHT(Sheet1!B178, 1) = ".", LEFT(Sheet1!B178, LEN(Sheet1!B178)-1),Sheet1!B178))</f>
+        <v>0</v>
+      </c>
+      <c r="H178" t="b">
+        <f>TRIM(C178)=TRIM(IF(RIGHT(Sheet1!C178, 1) = ".", LEFT(Sheet1!C178, LEN(Sheet1!C178)-1),Sheet1!C178))</f>
+        <v>0</v>
+      </c>
+      <c r="I178" t="b">
+        <f>TRIM(D178)=TRIM(IF(RIGHT(Sheet1!D178, 1) = ".", LEFT(Sheet1!D178, LEN(Sheet1!D178)-1),Sheet1!D178))</f>
+        <v>0</v>
+      </c>
+      <c r="J178" t="b">
+        <f>TRIM(E178)=TRIM(IF(RIGHT(Sheet1!E178, 1) = ".", LEFT(Sheet1!E178, LEN(Sheet1!E178)-1),Sheet1!E178))</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G177 G178:H178 H2:J2 H3:H177 I3:J178">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>